<commit_message>
reformatted code with black
</commit_message>
<xml_diff>
--- a/results/ppc_bus/va.xlsx
+++ b/results/ppc_bus/va.xlsx
@@ -412,31 +412,31 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-0.1730886903769808</v>
+        <v>-0.01132772767135682</v>
       </c>
       <c r="D2">
-        <v>-0.05492172868311176</v>
+        <v>0.1329501444668215</v>
       </c>
       <c r="E2">
-        <v>0.02911889389037105</v>
+        <v>0.2452044431023112</v>
       </c>
       <c r="F2">
-        <v>0.07888216210728016</v>
+        <v>0.3210583506375297</v>
       </c>
       <c r="G2">
-        <v>0.1138308094624324</v>
+        <v>0.3622452035370414</v>
       </c>
       <c r="H2">
-        <v>-0.02015030881098215</v>
+        <v>0.1654327651585601</v>
       </c>
       <c r="I2">
-        <v>0.06375830977882029</v>
+        <v>0.2818359714947122</v>
       </c>
       <c r="J2">
-        <v>0.09385202513880553</v>
+        <v>0.355822772016644</v>
       </c>
       <c r="K2">
-        <v>0.1488231498640391</v>
+        <v>0.4034558434828278</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -447,31 +447,31 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>-0.3920118456361024</v>
+        <v>0.04167199304037311</v>
       </c>
       <c r="D3">
-        <v>-0.3089241627190564</v>
+        <v>0.1945323064040473</v>
       </c>
       <c r="E3">
-        <v>-0.2601514133366861</v>
+        <v>0.315326141460165</v>
       </c>
       <c r="F3">
-        <v>-0.2529415190795412</v>
+        <v>0.3952634884591798</v>
       </c>
       <c r="G3">
-        <v>-0.241060372680467</v>
+        <v>0.4363374629815695</v>
       </c>
       <c r="H3">
-        <v>-0.2739381108365492</v>
+        <v>0.2269676979385108</v>
       </c>
       <c r="I3">
-        <v>-0.2183200689834985</v>
+        <v>0.3563520789343781</v>
       </c>
       <c r="J3">
-        <v>-0.2575686055570127</v>
+        <v>0.4342047310983628</v>
       </c>
       <c r="K3">
-        <v>-0.2291346678826717</v>
+        <v>0.4774351088200124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new EU LV analysis
</commit_message>
<xml_diff>
--- a/results/ppc_bus/va.xlsx
+++ b/results/ppc_bus/va.xlsx
@@ -412,66 +412,66 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-0.03073838356816078</v>
+        <v>-0.3955679064921799</v>
       </c>
       <c r="D2">
-        <v>0.1103953264405628</v>
+        <v>-0.3135526085529318</v>
       </c>
       <c r="E2">
-        <v>0.2203687944236038</v>
+        <v>-0.219670687897636</v>
       </c>
       <c r="F2">
-        <v>0.2984173663849913</v>
+        <v>-0.1582138509973569</v>
       </c>
       <c r="G2">
-        <v>0.3396271737463568</v>
+        <v>-0.1253459904459567</v>
       </c>
       <c r="H2">
-        <v>0.1420413390573121</v>
+        <v>-0.3248105319531392</v>
       </c>
       <c r="I2">
-        <v>0.2525333222225323</v>
+        <v>-0.186905187417177</v>
       </c>
       <c r="J2">
-        <v>0.3353444977170092</v>
+        <v>-0.1294736865881621</v>
       </c>
       <c r="K2">
-        <v>0.3808607917274153</v>
+        <v>-0.09242948704970184</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.001594388907581552</v>
+        <v>-0.4535728184682561</v>
       </c>
       <c r="D3">
-        <v>0.1479671853865113</v>
+        <v>-0.3809226417101971</v>
       </c>
       <c r="E3">
-        <v>0.2623073227449058</v>
+        <v>-0.3007008387427232</v>
       </c>
       <c r="F3">
-        <v>0.3357708147817765</v>
+        <v>-0.2529676474746937</v>
       </c>
       <c r="G3">
-        <v>0.3724482494876078</v>
+        <v>-0.2199545933085434</v>
       </c>
       <c r="H3">
-        <v>0.1804382791030193</v>
+        <v>-0.387860987107398</v>
       </c>
       <c r="I3">
-        <v>0.3034052846052124</v>
+        <v>-0.2678362558876907</v>
       </c>
       <c r="J3">
-        <v>0.3726650190200617</v>
+        <v>-0.2380870939725943</v>
       </c>
       <c r="K3">
-        <v>0.4091634066071575</v>
+        <v>-0.1868924887586276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some proper comments
</commit_message>
<xml_diff>
--- a/results/ppc_bus/va.xlsx
+++ b/results/ppc_bus/va.xlsx
@@ -5829,2722 +5829,2722 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>-0.07389476076042259</v>
+        <v>-0.07837925135774969</v>
       </c>
       <c r="D3">
-        <v>-0.07372340523960064</v>
+        <v>-0.07824841720318731</v>
       </c>
       <c r="E3">
-        <v>-0.07370543947482767</v>
+        <v>-0.07823469983275989</v>
       </c>
       <c r="F3">
-        <v>-0.07368860811056326</v>
+        <v>-0.07822184859769163</v>
       </c>
       <c r="G3">
-        <v>-0.07367393336968786</v>
+        <v>-0.07821064399803875</v>
       </c>
       <c r="H3">
-        <v>-0.07365081449769006</v>
+        <v>-0.07819299203671366</v>
       </c>
       <c r="I3">
-        <v>-0.07207539540065469</v>
+        <v>-0.07699006195004714</v>
       </c>
       <c r="J3">
-        <v>-0.07200478268177446</v>
+        <v>-0.07693614246900271</v>
       </c>
       <c r="K3">
-        <v>-0.07194600698157262</v>
+        <v>-0.07689126151967361</v>
       </c>
       <c r="L3">
-        <v>-0.07189442406457072</v>
+        <v>-0.07685187284571214</v>
       </c>
       <c r="M3">
-        <v>-0.07185593190235597</v>
+        <v>-0.07682248019311091</v>
       </c>
       <c r="N3">
-        <v>-0.07181979602461414</v>
+        <v>-0.07679488674837298</v>
       </c>
       <c r="O3">
-        <v>-0.07179757517808405</v>
+        <v>-0.07677791882993522</v>
       </c>
       <c r="P3">
-        <v>-0.07174225330454748</v>
+        <v>-0.07673567476334198</v>
       </c>
       <c r="Q3">
-        <v>-0.07129399872161109</v>
+        <v>-0.07639338080496461</v>
       </c>
       <c r="R3">
-        <v>-0.07129399872161069</v>
+        <v>-0.07639338080496189</v>
       </c>
       <c r="S3">
-        <v>-0.07075017172669568</v>
+        <v>-0.07597809565633074</v>
       </c>
       <c r="T3">
-        <v>-0.07129399872161081</v>
+        <v>-0.07639338080496065</v>
       </c>
       <c r="U3">
-        <v>-0.07071274336698821</v>
+        <v>-0.07594951363348651</v>
       </c>
       <c r="V3">
-        <v>-0.07129399872161102</v>
+        <v>-0.07639338080495955</v>
       </c>
       <c r="W3">
-        <v>-0.07067071419170999</v>
+        <v>-0.07591741814957995</v>
       </c>
       <c r="X3">
-        <v>-0.07129399872161099</v>
+        <v>-0.07639338080495871</v>
       </c>
       <c r="Y3">
-        <v>-0.07060227880373668</v>
+        <v>-0.07586515747222063</v>
       </c>
       <c r="Z3">
-        <v>-0.07129399872161098</v>
+        <v>-0.07639338080495855</v>
       </c>
       <c r="AA3">
-        <v>-0.07047776750431888</v>
+        <v>-0.07577007395606165</v>
       </c>
       <c r="AB3">
-        <v>-0.07129399872161113</v>
+        <v>-0.076393380804959</v>
       </c>
       <c r="AC3">
-        <v>-0.07013014198066103</v>
+        <v>-0.07549295317962089</v>
       </c>
       <c r="AD3">
-        <v>-0.06906246422658784</v>
+        <v>-0.07462760253092848</v>
       </c>
       <c r="AE3">
-        <v>-0.07129399872161139</v>
+        <v>-0.07639338080495961</v>
       </c>
       <c r="AF3">
-        <v>-0.07003023180497289</v>
+        <v>-0.07541246148955884</v>
       </c>
       <c r="AG3">
-        <v>-0.07013418950022769</v>
+        <v>-0.07549700163421393</v>
       </c>
       <c r="AH3">
-        <v>-0.06868536289473634</v>
+        <v>-0.07432318454370729</v>
       </c>
       <c r="AI3">
-        <v>-0.07129399872161198</v>
+        <v>-0.07639338080496222</v>
       </c>
       <c r="AJ3">
-        <v>-0.06980142922821941</v>
+        <v>-0.07522812616366156</v>
       </c>
       <c r="AK3">
-        <v>-0.07013432657062681</v>
+        <v>-0.07549713873627935</v>
       </c>
       <c r="AL3">
-        <v>-0.06885004063966398</v>
+        <v>-0.07454588556873223</v>
       </c>
       <c r="AM3">
-        <v>-0.06735785100913746</v>
+        <v>-0.07314994275047687</v>
       </c>
       <c r="AN3">
-        <v>-0.07129399872161206</v>
+        <v>-0.07639338080496476</v>
       </c>
       <c r="AO3">
-        <v>-0.07013452365315977</v>
+        <v>-0.07549733586434508</v>
       </c>
       <c r="AP3">
-        <v>-0.06885344880149183</v>
+        <v>-0.07455833013940451</v>
       </c>
       <c r="AQ3">
-        <v>-0.06888659806076769</v>
+        <v>-0.07455994459682361</v>
       </c>
       <c r="AR3">
-        <v>-0.06643582129903165</v>
+        <v>-0.07233503878874759</v>
       </c>
       <c r="AS3">
-        <v>-0.06735785100919602</v>
+        <v>-0.07314994275048317</v>
       </c>
       <c r="AT3">
-        <v>-0.07129399872161207</v>
+        <v>-0.07639338080496563</v>
       </c>
       <c r="AU3">
-        <v>-0.07013477639821743</v>
+        <v>-0.07549758866779485</v>
       </c>
       <c r="AV3">
-        <v>-0.06885498496375513</v>
+        <v>-0.07456393930292518</v>
       </c>
       <c r="AW3">
-        <v>-0.06897456463803739</v>
+        <v>-0.07459377365061087</v>
       </c>
       <c r="AX3">
-        <v>-0.06573863439297634</v>
+        <v>-0.07171884166432244</v>
       </c>
       <c r="AY3">
-        <v>-0.06735785100922176</v>
+        <v>-0.07314994275049339</v>
       </c>
       <c r="AZ3">
-        <v>-0.07129399872161182</v>
+        <v>-0.0763933808049662</v>
       </c>
       <c r="BA3">
-        <v>-0.07013539194701861</v>
+        <v>-0.07549820435880637</v>
       </c>
       <c r="BB3">
-        <v>-0.06885661296808299</v>
+        <v>-0.07456988383117316</v>
       </c>
       <c r="BC3">
-        <v>-0.06563808220379976</v>
+        <v>-0.07162996937329398</v>
       </c>
       <c r="BD3">
-        <v>-0.0657386343929451</v>
+        <v>-0.07171884166430846</v>
       </c>
       <c r="BE3">
-        <v>-0.06735785100924545</v>
+        <v>-0.07314994275050565</v>
       </c>
       <c r="BF3">
-        <v>-0.07129399872161103</v>
+        <v>-0.07639338080496751</v>
       </c>
       <c r="BG3">
-        <v>-0.07013591897001815</v>
+        <v>-0.07549873150356459</v>
       </c>
       <c r="BH3">
-        <v>-0.06885816353067174</v>
+        <v>-0.07457554559795353</v>
       </c>
       <c r="BI3">
-        <v>-0.06518250666554558</v>
+        <v>-0.07122730953925709</v>
       </c>
       <c r="BJ3">
-        <v>-0.06573863439294354</v>
+        <v>-0.07171884166430861</v>
       </c>
       <c r="BK3">
-        <v>-0.06735785100925605</v>
+        <v>-0.07314994275051999</v>
       </c>
       <c r="BL3">
-        <v>-0.07129399872160981</v>
+        <v>-0.0763933808049687</v>
       </c>
       <c r="BM3">
-        <v>-0.07013844534007253</v>
+        <v>-0.07550125845729154</v>
       </c>
       <c r="BN3">
-        <v>-0.06885909216482498</v>
+        <v>-0.07457893644326366</v>
       </c>
       <c r="BO3">
-        <v>-0.06508573282292879</v>
+        <v>-0.07113715671262383</v>
       </c>
       <c r="BP3">
-        <v>-0.0651277072060551</v>
+        <v>-0.07124827836832918</v>
       </c>
       <c r="BQ3">
-        <v>-0.06573863439294293</v>
+        <v>-0.07171884166430932</v>
       </c>
       <c r="BR3">
-        <v>-0.06735785100927039</v>
+        <v>-0.07314994275052718</v>
       </c>
       <c r="BS3">
-        <v>-0.07129399872160766</v>
+        <v>-0.07639338080496999</v>
       </c>
       <c r="BT3">
-        <v>-0.0701473753348658</v>
+        <v>-0.07551019051523031</v>
       </c>
       <c r="BU3">
-        <v>-0.0688609140780049</v>
+        <v>-0.07458558904807597</v>
       </c>
       <c r="BV3">
-        <v>-0.06394186305152148</v>
+        <v>-0.07007153767938182</v>
       </c>
       <c r="BW3">
-        <v>-0.06505405824325904</v>
+        <v>-0.07117381231848982</v>
       </c>
       <c r="BX3">
-        <v>-0.06517456947073634</v>
+        <v>-0.07133299586877773</v>
       </c>
       <c r="BY3">
-        <v>-0.06573863439294088</v>
+        <v>-0.07171884166431307</v>
       </c>
       <c r="BZ3">
-        <v>-0.06735785100929169</v>
+        <v>-0.07314994275053686</v>
       </c>
       <c r="CA3">
-        <v>-0.07129399872159815</v>
+        <v>-0.07639338080497518</v>
       </c>
       <c r="CB3">
-        <v>-0.06887014762721379</v>
+        <v>-0.07461930501506203</v>
       </c>
       <c r="CC3">
-        <v>-0.06354291294763052</v>
+        <v>-0.06969987498422608</v>
       </c>
       <c r="CD3">
-        <v>-0.06573863439293873</v>
+        <v>-0.07171884166431132</v>
       </c>
       <c r="CE3">
-        <v>-0.06735785100934978</v>
+        <v>-0.07314994275056565</v>
       </c>
       <c r="CF3">
-        <v>-0.07129399872158579</v>
+        <v>-0.07639338080498173</v>
       </c>
       <c r="CG3">
-        <v>-0.06890494204975944</v>
+        <v>-0.07474635895838136</v>
       </c>
       <c r="CH3">
-        <v>-0.06345583338898007</v>
+        <v>-0.06961875120304357</v>
       </c>
       <c r="CI3">
-        <v>-0.06573863439294089</v>
+        <v>-0.07171884166431029</v>
       </c>
       <c r="CJ3">
-        <v>-0.06735785100945908</v>
+        <v>-0.07314994275061895</v>
       </c>
       <c r="CK3">
-        <v>-0.07129399872157874</v>
+        <v>-0.07639338080498573</v>
       </c>
       <c r="CL3">
-        <v>-0.06327923263653706</v>
+        <v>-0.06945422867638479</v>
       </c>
       <c r="CM3">
-        <v>-0.06573863439294089</v>
+        <v>-0.07171884166431029</v>
       </c>
       <c r="CN3">
-        <v>-0.06735785100948252</v>
+        <v>-0.07314994275063488</v>
       </c>
       <c r="CO3">
-        <v>-0.07129399872157635</v>
+        <v>-0.07639338080498763</v>
       </c>
       <c r="CP3">
-        <v>-0.06311266887729595</v>
+        <v>-0.06929905628686868</v>
       </c>
       <c r="CQ3">
-        <v>-0.06735785100948058</v>
+        <v>-0.07314994275063549</v>
       </c>
       <c r="CR3">
-        <v>-0.07129399872157582</v>
+        <v>-0.07639338080498766</v>
       </c>
       <c r="CS3">
-        <v>-0.06301584640239684</v>
+        <v>-0.06920885536676008</v>
       </c>
       <c r="CT3">
-        <v>-0.0673578510094775</v>
+        <v>-0.0731499427506343</v>
       </c>
       <c r="CU3">
-        <v>-0.0712939987215757</v>
+        <v>-0.07639338080498785</v>
       </c>
       <c r="CV3">
-        <v>-0.06295189860434293</v>
+        <v>-0.06914928079841196</v>
       </c>
       <c r="CW3">
-        <v>-0.06735785100948395</v>
+        <v>-0.07314994275063651</v>
       </c>
       <c r="CX3">
-        <v>-0.07129399872157582</v>
+        <v>-0.07639338080498817</v>
       </c>
       <c r="CY3">
-        <v>-0.0628635995851916</v>
+        <v>-0.0690670202344454</v>
       </c>
       <c r="CZ3">
-        <v>-0.06735785101002652</v>
+        <v>-0.07314994275104843</v>
       </c>
       <c r="DA3">
-        <v>-0.07129399872157582</v>
+        <v>-0.07639338080498817</v>
       </c>
       <c r="DB3">
-        <v>-0.06287641873746179</v>
+        <v>-0.06908487090211386</v>
       </c>
       <c r="DC3">
-        <v>-0.06279120461877945</v>
+        <v>-0.06899244727468042</v>
       </c>
       <c r="DD3">
-        <v>-0.06735785101005014</v>
+        <v>-0.07314994275106634</v>
       </c>
       <c r="DE3">
-        <v>-0.06289192815396404</v>
+        <v>-0.06910646776787194</v>
       </c>
       <c r="DF3">
-        <v>-0.06275015181758256</v>
+        <v>-0.06895015942112441</v>
       </c>
       <c r="DG3">
-        <v>-0.0673578510101067</v>
+        <v>-0.07314994275110641</v>
       </c>
       <c r="DH3">
-        <v>-0.06290990468831693</v>
+        <v>-0.06913150010335212</v>
       </c>
       <c r="DI3">
-        <v>-0.06112958660714583</v>
+        <v>-0.06728084956105333</v>
       </c>
       <c r="DJ3">
-        <v>-0.06735785101160147</v>
+        <v>-0.07314994275224107</v>
       </c>
       <c r="DK3">
-        <v>-0.06293731360034245</v>
+        <v>-0.06916966704637734</v>
       </c>
       <c r="DL3">
-        <v>-0.06096716262379215</v>
+        <v>-0.06711354105137506</v>
       </c>
       <c r="DM3">
-        <v>-0.06735785101293151</v>
+        <v>-0.0731499427532501</v>
       </c>
       <c r="DN3">
-        <v>-0.06297255152216838</v>
+        <v>-0.06921873592273947</v>
       </c>
       <c r="DO3">
-        <v>-0.06103261162003996</v>
+        <v>-0.06715825307045066</v>
       </c>
       <c r="DP3">
-        <v>-0.06104283911357485</v>
+        <v>-0.06723890368142124</v>
       </c>
       <c r="DQ3">
-        <v>-0.06735785101305712</v>
+        <v>-0.0731499427533404</v>
       </c>
       <c r="DR3">
-        <v>-0.06299784901901698</v>
+        <v>-0.06925396275676843</v>
       </c>
       <c r="DS3">
-        <v>-0.06103261162004066</v>
+        <v>-0.06715825307045167</v>
       </c>
       <c r="DT3">
-        <v>-0.06106447841585751</v>
+        <v>-0.06718002311817722</v>
       </c>
       <c r="DU3">
-        <v>-0.06117935724609731</v>
+        <v>-0.06746505619398938</v>
       </c>
       <c r="DV3">
-        <v>-0.06735785101315538</v>
+        <v>-0.073149942753405</v>
       </c>
       <c r="DW3">
-        <v>-0.06303359424710964</v>
+        <v>-0.06930373811277801</v>
       </c>
       <c r="DX3">
-        <v>-0.06103261162004134</v>
+        <v>-0.06715825307045263</v>
       </c>
       <c r="DY3">
-        <v>-0.06121417860380719</v>
+        <v>-0.06728229182258862</v>
       </c>
       <c r="DZ3">
-        <v>-0.06124076845413077</v>
+        <v>-0.06756678932604777</v>
       </c>
       <c r="EA3">
-        <v>-0.06735785101323956</v>
+        <v>-0.07314994275346702</v>
       </c>
       <c r="EB3">
-        <v>-0.06307226808251366</v>
+        <v>-0.06935759160096017</v>
       </c>
       <c r="EC3">
-        <v>-0.06103261162004119</v>
+        <v>-0.06715825307045289</v>
       </c>
       <c r="ED3">
-        <v>-0.06115198895122473</v>
+        <v>-0.06725000490485626</v>
       </c>
       <c r="EE3">
-        <v>-0.06160940407061749</v>
+        <v>-0.06749974096192367</v>
       </c>
       <c r="EF3">
-        <v>-0.06125904225942567</v>
+        <v>-0.06759706161472942</v>
       </c>
       <c r="EG3">
-        <v>-0.06735785101349298</v>
+        <v>-0.07314994275365301</v>
       </c>
       <c r="EH3">
-        <v>-0.06310874068705997</v>
+        <v>-0.06940837989983281</v>
       </c>
       <c r="EI3">
-        <v>-0.06103261162004107</v>
+        <v>-0.06715825307045359</v>
       </c>
       <c r="EJ3">
-        <v>-0.06114663316617588</v>
+        <v>-0.06724722432856269</v>
       </c>
       <c r="EK3">
-        <v>-0.06190343551862033</v>
+        <v>-0.06766151299970211</v>
       </c>
       <c r="EL3">
-        <v>-0.06127967102793586</v>
+        <v>-0.067631235180118</v>
       </c>
       <c r="EM3">
-        <v>-0.06735785101368093</v>
+        <v>-0.07314994275378928</v>
       </c>
       <c r="EN3">
-        <v>-0.06316870760721752</v>
+        <v>-0.06949188423286479</v>
       </c>
       <c r="EO3">
-        <v>-0.06103261162004015</v>
+        <v>-0.06715825307045394</v>
       </c>
       <c r="EP3">
-        <v>-0.06114137811740254</v>
+        <v>-0.06724449604859191</v>
       </c>
       <c r="EQ3">
-        <v>-0.06210034334449402</v>
+        <v>-0.06776984841275231</v>
       </c>
       <c r="ER3">
-        <v>-0.06129907322541175</v>
+        <v>-0.06766337686638299</v>
       </c>
       <c r="ES3">
-        <v>-0.06735785101371161</v>
+        <v>-0.07314994275381258</v>
       </c>
       <c r="ET3">
-        <v>-0.06345383956286407</v>
+        <v>-0.0698889336050014</v>
       </c>
       <c r="EU3">
-        <v>-0.06103261162003944</v>
+        <v>-0.06715825307045389</v>
       </c>
       <c r="EV3">
-        <v>-0.06113713488360147</v>
+        <v>-0.06724229307344248</v>
       </c>
       <c r="EW3">
-        <v>-0.06227568009595016</v>
+        <v>-0.06781274052429591</v>
       </c>
       <c r="EX3">
-        <v>-0.06213784216234119</v>
+        <v>-0.06788974889235148</v>
       </c>
       <c r="EY3">
-        <v>-0.06132171337716145</v>
+        <v>-0.06770088261648957</v>
       </c>
       <c r="EZ3">
-        <v>-0.06735785101371598</v>
+        <v>-0.07314994275382257</v>
       </c>
       <c r="FA3">
-        <v>-0.06351595458956273</v>
+        <v>-0.06997542973148901</v>
       </c>
       <c r="FB3">
-        <v>-0.06103261162003901</v>
+        <v>-0.0671582530704542</v>
       </c>
       <c r="FC3">
-        <v>-0.06113076611925846</v>
+        <v>-0.06723898657500502</v>
       </c>
       <c r="FD3">
-        <v>-0.06274069043541158</v>
+        <v>-0.06792649336383288</v>
       </c>
       <c r="FE3">
-        <v>-0.06214012460361183</v>
+        <v>-0.06789704702266093</v>
       </c>
       <c r="FF3">
-        <v>-0.06132822826098978</v>
+        <v>-0.06771167520807536</v>
       </c>
       <c r="FG3">
-        <v>-0.06735785101371856</v>
+        <v>-0.07314994275381996</v>
       </c>
       <c r="FH3">
-        <v>-0.06356294535380821</v>
+        <v>-0.07035205464923629</v>
       </c>
       <c r="FI3">
-        <v>-0.06373462259844311</v>
+        <v>-0.07017251044344577</v>
       </c>
       <c r="FJ3">
-        <v>-0.0610326116200381</v>
+        <v>-0.06715825307045396</v>
       </c>
       <c r="FK3">
-        <v>-0.06112308785020473</v>
+        <v>-0.067235000209296</v>
       </c>
       <c r="FL3">
-        <v>-0.06290221626343991</v>
+        <v>-0.06796600607988747</v>
       </c>
       <c r="FM3">
-        <v>-0.06214220973683054</v>
+        <v>-0.06790371427296339</v>
       </c>
       <c r="FN3">
-        <v>-0.0613652428854503</v>
+        <v>-0.06777299394879918</v>
       </c>
       <c r="FO3">
-        <v>-0.06735785101371855</v>
+        <v>-0.07314994275381996</v>
       </c>
       <c r="FP3">
-        <v>-0.0635718228167301</v>
+        <v>-0.07042321273034131</v>
       </c>
       <c r="FQ3">
-        <v>-0.06402493105296572</v>
+        <v>-0.07043415882562765</v>
       </c>
       <c r="FR3">
-        <v>-0.06103261162003655</v>
+        <v>-0.06715825307045384</v>
       </c>
       <c r="FS3">
-        <v>-0.06111728706838079</v>
+        <v>-0.06723198858365421</v>
       </c>
       <c r="FT3">
-        <v>-0.06290221626309718</v>
+        <v>-0.0679660060795407</v>
       </c>
       <c r="FU3">
-        <v>-0.06317106949358819</v>
+        <v>-0.06803159573160167</v>
       </c>
       <c r="FV3">
-        <v>-0.06214307593043113</v>
+        <v>-0.06790648394639995</v>
       </c>
       <c r="FW3">
-        <v>-0.06138615086529393</v>
+        <v>-0.06780763037175806</v>
       </c>
       <c r="FX3">
-        <v>-0.0635901389253765</v>
+        <v>-0.07057003349046803</v>
       </c>
       <c r="FY3">
-        <v>-0.06405259688870932</v>
+        <v>-0.0704640816696649</v>
       </c>
       <c r="FZ3">
-        <v>-0.06408090094323989</v>
+        <v>-0.07047119772666756</v>
       </c>
       <c r="GA3">
-        <v>-0.0610326116200347</v>
+        <v>-0.06715825307045338</v>
       </c>
       <c r="GB3">
-        <v>-0.06111057454465681</v>
+        <v>-0.06722850359887876</v>
       </c>
       <c r="GC3">
-        <v>-0.06290221626306054</v>
+        <v>-0.06796600607948865</v>
       </c>
       <c r="GD3">
-        <v>-0.0632001078738811</v>
+        <v>-0.06803867959445878</v>
       </c>
       <c r="GE3">
-        <v>-0.06214494300175644</v>
+        <v>-0.0679124539569517</v>
       </c>
       <c r="GF3">
-        <v>-0.06140167232026189</v>
+        <v>-0.06783334344999224</v>
       </c>
       <c r="GG3">
-        <v>-0.06416146973726661</v>
+        <v>-0.07058183651117377</v>
       </c>
       <c r="GH3">
-        <v>-0.0643125638853293</v>
+        <v>-0.0706245006963421</v>
       </c>
       <c r="GI3">
-        <v>-0.06103261162003336</v>
+        <v>-0.06715825307045246</v>
       </c>
       <c r="GJ3">
-        <v>-0.06110426303106267</v>
+        <v>-0.06722522680446373</v>
       </c>
       <c r="GK3">
-        <v>-0.06290221626306083</v>
+        <v>-0.06796600607948894</v>
       </c>
       <c r="GL3">
-        <v>-0.06290221626304579</v>
+        <v>-0.06796600607946389</v>
       </c>
       <c r="GM3">
-        <v>-0.06322819634509655</v>
+        <v>-0.06804553166113296</v>
       </c>
       <c r="GN3">
-        <v>-0.06214969841761907</v>
+        <v>-0.0679276595769623</v>
       </c>
       <c r="GO3">
-        <v>-0.0614156274754736</v>
+        <v>-0.06785646180156148</v>
       </c>
       <c r="GP3">
-        <v>-0.06435585842190489</v>
+        <v>-0.07079208380506063</v>
       </c>
       <c r="GQ3">
-        <v>-0.06432725381698799</v>
+        <v>-0.07063919587711813</v>
       </c>
       <c r="GR3">
-        <v>-0.06433024360543985</v>
+        <v>-0.07063332511460217</v>
       </c>
       <c r="GS3">
-        <v>-0.06103261162003259</v>
+        <v>-0.06715825307045246</v>
       </c>
       <c r="GT3">
-        <v>-0.0610974722037309</v>
+        <v>-0.06722170115617876</v>
       </c>
       <c r="GU3">
-        <v>-0.06290221626306083</v>
+        <v>-0.06796600607948894</v>
       </c>
       <c r="GV3">
-        <v>-0.06290221626303383</v>
+        <v>-0.06796600607944929</v>
       </c>
       <c r="GW3">
-        <v>-0.06325066456656847</v>
+        <v>-0.06805101264328227</v>
       </c>
       <c r="GX3">
-        <v>-0.06215248840128624</v>
+        <v>-0.06793658068778653</v>
       </c>
       <c r="GY3">
-        <v>-0.0614329645885095</v>
+        <v>-0.06788518280162907</v>
       </c>
       <c r="GZ3">
-        <v>-0.06433374517468327</v>
+        <v>-0.07079410056190774</v>
       </c>
       <c r="HA3">
-        <v>-0.06439491083182143</v>
+        <v>-0.07082302764914132</v>
       </c>
       <c r="HB3">
-        <v>-0.06436439405355823</v>
+        <v>-0.07067634938508359</v>
       </c>
       <c r="HC3">
-        <v>-0.06433274266298322</v>
+        <v>-0.07063457245777548</v>
       </c>
       <c r="HD3">
-        <v>-0.06103261162003171</v>
+        <v>-0.06715825307045255</v>
       </c>
       <c r="HE3">
-        <v>-0.06108709104700253</v>
+        <v>-0.06721631147762772</v>
       </c>
       <c r="HF3">
-        <v>-0.06290221626301626</v>
+        <v>-0.06796600607944168</v>
       </c>
       <c r="HG3">
-        <v>-0.06326856244144402</v>
+        <v>-0.06805537868756267</v>
       </c>
       <c r="HH3">
-        <v>-0.06215444251750409</v>
+        <v>-0.06794282908593952</v>
       </c>
       <c r="HI3">
-        <v>-0.0614649598160538</v>
+        <v>-0.06793818683291618</v>
       </c>
       <c r="HJ3">
-        <v>-0.06426136366685807</v>
+        <v>-0.07080070200473662</v>
       </c>
       <c r="HK3">
-        <v>-0.06446539392623032</v>
+        <v>-0.07087887610376344</v>
       </c>
       <c r="HL3">
-        <v>-0.0643347580842771</v>
+        <v>-0.07063557840527804</v>
       </c>
       <c r="HM3">
-        <v>-0.06103261162003169</v>
+        <v>-0.06715825307045253</v>
       </c>
       <c r="HN3">
-        <v>-0.06105874109903288</v>
+        <v>-0.06720159271745089</v>
       </c>
       <c r="HO3">
-        <v>-0.06290221626300375</v>
+        <v>-0.06796600607944547</v>
       </c>
       <c r="HP3">
-        <v>-0.06330640189736256</v>
+        <v>-0.06806460923327345</v>
       </c>
       <c r="HQ3">
-        <v>-0.06215820145591454</v>
+        <v>-0.06795484854049609</v>
       </c>
       <c r="HR3">
-        <v>-0.06149285719742207</v>
+        <v>-0.06798440239681358</v>
       </c>
       <c r="HS3">
-        <v>-0.06423016030809768</v>
+        <v>-0.07080354793196192</v>
       </c>
       <c r="HT3">
-        <v>-0.06449056038146245</v>
+        <v>-0.07089881715491859</v>
       </c>
       <c r="HU3">
-        <v>-0.06433636870550456</v>
+        <v>-0.07063638230654422</v>
       </c>
       <c r="HV3">
-        <v>-0.06105632388283869</v>
+        <v>-0.06720033773999284</v>
       </c>
       <c r="HW3">
-        <v>-0.06290221626300199</v>
+        <v>-0.06796600607945176</v>
       </c>
       <c r="HX3">
-        <v>-0.06333620183125445</v>
+        <v>-0.0680718785355669</v>
       </c>
       <c r="HY3">
-        <v>-0.06216007241407082</v>
+        <v>-0.06796083107001058</v>
       </c>
       <c r="HZ3">
-        <v>-0.06151183569298829</v>
+        <v>-0.06801584275427607</v>
       </c>
       <c r="IA3">
-        <v>-0.06477044138718141</v>
+        <v>-0.07111986000854638</v>
       </c>
       <c r="IB3">
-        <v>-0.06449056038146245</v>
+        <v>-0.07089881715491859</v>
       </c>
       <c r="IC3">
-        <v>-0.06433882733650993</v>
+        <v>-0.07063760947009146</v>
       </c>
       <c r="ID3">
-        <v>-0.06105520739288709</v>
+        <v>-0.06719975807721006</v>
       </c>
       <c r="IE3">
-        <v>-0.06290221626300459</v>
+        <v>-0.06796600607945423</v>
       </c>
       <c r="IF3">
-        <v>-0.06335687278884113</v>
+        <v>-0.06807692090016348</v>
       </c>
       <c r="IG3">
-        <v>-0.06216140091093187</v>
+        <v>-0.067965079045518</v>
       </c>
       <c r="IH3">
-        <v>-0.06152430355360824</v>
+        <v>-0.06803649742225253</v>
       </c>
       <c r="II3">
-        <v>-0.06481108925064955</v>
+        <v>-0.07115196215720287</v>
       </c>
       <c r="IJ3">
-        <v>-0.06434170935095221</v>
+        <v>-0.07063904795390551</v>
       </c>
       <c r="IK3">
-        <v>-0.0610540131714234</v>
+        <v>-0.06719913805737877</v>
       </c>
       <c r="IL3">
-        <v>-0.06290221626300498</v>
+        <v>-0.06796600607945275</v>
       </c>
       <c r="IM3">
-        <v>-0.06337749469685355</v>
+        <v>-0.0680819512640476</v>
       </c>
       <c r="IN3">
-        <v>-0.06217659840894387</v>
+        <v>-0.06801367466960562</v>
       </c>
       <c r="IO3">
-        <v>-0.06155113816505876</v>
+        <v>-0.06808095259730659</v>
       </c>
       <c r="IP3">
-        <v>-0.0648923400282381</v>
+        <v>-0.07119382570876669</v>
       </c>
       <c r="IQ3">
-        <v>-0.06485460895676658</v>
+        <v>-0.07120863702672814</v>
       </c>
       <c r="IR3">
-        <v>-0.06434613596137463</v>
+        <v>-0.07064125738146125</v>
       </c>
       <c r="IS3">
-        <v>-0.06105287203992765</v>
+        <v>-0.06719854560082054</v>
       </c>
       <c r="IT3">
-        <v>-0.06290221626301065</v>
+        <v>-0.06796600607945971</v>
       </c>
       <c r="IU3">
-        <v>-0.0634076639786636</v>
+        <v>-0.06808931048301077</v>
       </c>
       <c r="IV3">
-        <v>-0.06218107992390668</v>
+        <v>-0.06802800493398341</v>
       </c>
       <c r="IW3">
-        <v>-0.06156331134955013</v>
+        <v>-0.06818619627011553</v>
       </c>
       <c r="IX3">
-        <v>-0.0615643875021896</v>
+        <v>-0.06809136589044312</v>
       </c>
       <c r="IY3">
-        <v>-0.06436233441832706</v>
+        <v>-0.07064934240124474</v>
       </c>
       <c r="IZ3">
-        <v>-0.06105160077019516</v>
+        <v>-0.06719788557847299</v>
       </c>
       <c r="JA3">
-        <v>-0.06290221626301119</v>
+        <v>-0.06796600607947575</v>
       </c>
       <c r="JB3">
-        <v>-0.06352113587251045</v>
+        <v>-0.0681169890944837</v>
       </c>
       <c r="JC3">
-        <v>-0.0621820825732155</v>
+        <v>-0.06803121105273641</v>
       </c>
       <c r="JD3">
-        <v>-0.06156499412432778</v>
+        <v>-0.0682007451071584</v>
       </c>
       <c r="JE3">
-        <v>-0.06161407706598709</v>
+        <v>-0.06813041928069959</v>
       </c>
       <c r="JF3">
-        <v>-0.06444117403125463</v>
+        <v>-0.07068869262529491</v>
       </c>
       <c r="JG3">
-        <v>-0.06104897669008751</v>
+        <v>-0.06719652319863363</v>
       </c>
       <c r="JH3">
-        <v>-0.0629022162630138</v>
+        <v>-0.06796600607948955</v>
       </c>
       <c r="JI3">
-        <v>-0.0635476211693107</v>
+        <v>-0.06812344935987327</v>
       </c>
       <c r="JJ3">
-        <v>-0.06220827733905523</v>
+        <v>-0.06808450177793121</v>
       </c>
       <c r="JK3">
-        <v>-0.06218205080997537</v>
+        <v>-0.06803215559017065</v>
       </c>
       <c r="JL3">
-        <v>-0.06156576775901249</v>
+        <v>-0.06820743378191221</v>
       </c>
       <c r="JM3">
-        <v>-0.06166392093328941</v>
+        <v>-0.06819865069957765</v>
       </c>
       <c r="JN3">
-        <v>-0.06162024849997669</v>
+        <v>-0.0681291481702746</v>
       </c>
       <c r="JO3">
-        <v>-0.06104624372585947</v>
+        <v>-0.06719510428709193</v>
       </c>
       <c r="JP3">
-        <v>-0.06290221626301795</v>
+        <v>-0.06796600607949874</v>
       </c>
       <c r="JQ3">
-        <v>-0.06355975488063485</v>
+        <v>-0.0681264089821082</v>
       </c>
       <c r="JR3">
-        <v>-0.06223423758173165</v>
+        <v>-0.06813731603816445</v>
       </c>
       <c r="JS3">
-        <v>-0.06218201356957668</v>
+        <v>-0.06803326300141195</v>
       </c>
       <c r="JT3">
-        <v>-0.06156668661635877</v>
+        <v>-0.06821537804322338</v>
       </c>
       <c r="JU3">
-        <v>-0.06166754407961848</v>
+        <v>-0.06820361045772422</v>
       </c>
       <c r="JV3">
-        <v>-0.06164262345745004</v>
+        <v>-0.06812453968141707</v>
       </c>
       <c r="JW3">
-        <v>-0.06103585122039056</v>
+        <v>-0.06718970865583719</v>
       </c>
       <c r="JX3">
-        <v>-0.06290221626300867</v>
+        <v>-0.06796600607950175</v>
       </c>
       <c r="JY3">
-        <v>-0.06356773191606598</v>
+        <v>-0.06812835471239201</v>
       </c>
       <c r="JZ3">
-        <v>-0.06218197991461642</v>
+        <v>-0.06803426379358955</v>
       </c>
       <c r="KA3">
-        <v>-0.0615681043054736</v>
+        <v>-0.06822763515661322</v>
       </c>
       <c r="KB3">
-        <v>-0.06167053039469503</v>
+        <v>-0.06820769845401838</v>
       </c>
       <c r="KC3">
-        <v>-0.06077721750781134</v>
+        <v>-0.06731760341947692</v>
       </c>
       <c r="KD3">
-        <v>-0.06186595552158424</v>
+        <v>-0.06831183879387832</v>
       </c>
       <c r="KE3">
-        <v>-0.06098067552176351</v>
+        <v>-0.06716106206353074</v>
       </c>
       <c r="KF3">
-        <v>-0.06290221626300867</v>
+        <v>-0.06796600607950175</v>
       </c>
       <c r="KG3">
-        <v>-0.06357454255052693</v>
+        <v>-0.06813516604052994</v>
       </c>
       <c r="KH3">
-        <v>-0.06357380400862009</v>
+        <v>-0.06812920056740319</v>
       </c>
       <c r="KI3">
-        <v>-0.06218194582886941</v>
+        <v>-0.06803527739647389</v>
       </c>
       <c r="KJ3">
-        <v>-0.06156936756847477</v>
+        <v>-0.06823855717757489</v>
       </c>
       <c r="KK3">
-        <v>-0.0616747722319554</v>
+        <v>-0.06821350515059887</v>
       </c>
       <c r="KL3">
-        <v>-0.06037887413354483</v>
+        <v>-0.06694616994719409</v>
       </c>
       <c r="KM3">
-        <v>-0.06280202789157277</v>
+        <v>-0.06909687324344702</v>
       </c>
       <c r="KN3">
-        <v>-0.06357767107466659</v>
+        <v>-0.06813829488331757</v>
       </c>
       <c r="KO3">
-        <v>-0.06357810145538864</v>
+        <v>-0.06812979920938018</v>
       </c>
       <c r="KP3">
-        <v>-0.06218190917979848</v>
+        <v>-0.06803636722504777</v>
       </c>
       <c r="KQ3">
-        <v>-0.06157034972831547</v>
+        <v>-0.0682470488474667</v>
       </c>
       <c r="KR3">
-        <v>-0.06169382475341813</v>
+        <v>-0.06823958640294873</v>
       </c>
       <c r="KS3">
-        <v>-0.05777638615557642</v>
+        <v>-0.06451943763761109</v>
       </c>
       <c r="KT3">
-        <v>-0.0630086765118197</v>
+        <v>-0.06927017642081104</v>
       </c>
       <c r="KU3">
-        <v>-0.06358296605464994</v>
+        <v>-0.0681435904026101</v>
       </c>
       <c r="KV3">
-        <v>-0.06358310242754978</v>
+        <v>-0.0681304958524251</v>
       </c>
       <c r="KW3">
-        <v>-0.06218169663552819</v>
+        <v>-0.06804268763688649</v>
       </c>
       <c r="KX3">
-        <v>-0.06157157227293118</v>
+        <v>-0.0682576189041994</v>
       </c>
       <c r="KY3">
-        <v>-0.06169749258491844</v>
+        <v>-0.06824460735631452</v>
       </c>
       <c r="KZ3">
-        <v>-0.05758198417679288</v>
+        <v>-0.0643381605720495</v>
       </c>
       <c r="LA3">
-        <v>-0.06307734332414716</v>
+        <v>-0.06932776278130642</v>
       </c>
       <c r="LB3">
-        <v>-0.06359312946086512</v>
+        <v>-0.06815375484400145</v>
       </c>
       <c r="LC3">
-        <v>-0.06359266771960013</v>
+        <v>-0.06813182830837947</v>
       </c>
       <c r="LD3">
-        <v>-0.06218079765366733</v>
+        <v>-0.06806942079623986</v>
       </c>
       <c r="LE3">
-        <v>-0.061572836742607</v>
+        <v>-0.06826855149022436</v>
       </c>
       <c r="LF3">
-        <v>-0.06170020831655288</v>
+        <v>-0.06824832496689974</v>
       </c>
       <c r="LG3">
-        <v>-0.05758458525295138</v>
+        <v>-0.06434382111500056</v>
       </c>
       <c r="LH3">
-        <v>-0.05395735193856145</v>
+        <v>-0.06092486239429912</v>
       </c>
       <c r="LI3">
-        <v>-0.06311318290094214</v>
+        <v>-0.06935781905488841</v>
       </c>
       <c r="LJ3">
-        <v>-0.06362305251646928</v>
+        <v>-0.06818368094739335</v>
       </c>
       <c r="LK3">
-        <v>-0.06362935266518593</v>
+        <v>-0.0681369385162206</v>
       </c>
       <c r="LL3">
-        <v>-0.06157432825595555</v>
+        <v>-0.0682814471544408</v>
       </c>
       <c r="LM3">
-        <v>-0.06170333654915856</v>
+        <v>-0.06825260725909056</v>
       </c>
       <c r="LN3">
-        <v>-0.05759798177618016</v>
+        <v>-0.06437297517137774</v>
       </c>
       <c r="LO3">
-        <v>-0.052217630968115</v>
+        <v>-0.05928651920729684</v>
       </c>
       <c r="LP3">
-        <v>-0.06314386287407669</v>
+        <v>-0.06938354829325767</v>
       </c>
       <c r="LQ3">
-        <v>-0.06375454908930174</v>
+        <v>-0.06815437780662166</v>
       </c>
       <c r="LR3">
-        <v>-0.061575178221383</v>
+        <v>-0.06828879600822721</v>
       </c>
       <c r="LS3">
-        <v>-0.06170643971529067</v>
+        <v>-0.06825685523957727</v>
       </c>
       <c r="LT3">
-        <v>-0.0576026588345994</v>
+        <v>-0.06438315362472737</v>
       </c>
       <c r="LU3">
-        <v>-0.05225305511421487</v>
+        <v>-0.05942959478845199</v>
       </c>
       <c r="LV3">
-        <v>-0.04884276652847062</v>
+        <v>-0.05603990227972357</v>
       </c>
       <c r="LW3">
-        <v>-0.06317875604366989</v>
+        <v>-0.06941281083688271</v>
       </c>
       <c r="LX3">
-        <v>-0.06157901803537655</v>
+        <v>-0.06832199554959137</v>
       </c>
       <c r="LY3">
-        <v>-0.06173370156323965</v>
+        <v>-0.06829417457377786</v>
       </c>
       <c r="LZ3">
-        <v>-0.05761283828799613</v>
+        <v>-0.06440530675938756</v>
       </c>
       <c r="MA3">
-        <v>-0.05226708499248896</v>
+        <v>-0.05948626240092664</v>
       </c>
       <c r="MB3">
-        <v>-0.04908848627332149</v>
+        <v>-0.05636065429132795</v>
       </c>
       <c r="MC3">
-        <v>-0.04819193779459025</v>
+        <v>-0.05540098211636714</v>
       </c>
       <c r="MD3">
-        <v>-0.06320624600402124</v>
+        <v>-0.06943586479386263</v>
       </c>
       <c r="ME3">
-        <v>-0.06158051241660364</v>
+        <v>-0.06833491628819316</v>
       </c>
       <c r="MF3">
-        <v>-0.06178942949194877</v>
+        <v>-0.06837046227519944</v>
       </c>
       <c r="MG3">
-        <v>-0.05761696131396928</v>
+        <v>-0.06442660121746069</v>
       </c>
       <c r="MH3">
-        <v>-0.05761482447167964</v>
+        <v>-0.06440383182162375</v>
       </c>
       <c r="MI3">
-        <v>-0.0492120334296101</v>
+        <v>-0.05652193159564433</v>
       </c>
       <c r="MJ3">
-        <v>-0.04763435526453872</v>
+        <v>-0.05485360060671017</v>
       </c>
       <c r="MK3">
-        <v>-0.0632292935364276</v>
+        <v>-0.06945519317879653</v>
       </c>
       <c r="ML3">
-        <v>-0.06158103156393904</v>
+        <v>-0.06833940496246345</v>
       </c>
       <c r="MM3">
-        <v>-0.05762313066223095</v>
+        <v>-0.06445846475975632</v>
       </c>
       <c r="MN3">
-        <v>-0.05761510102949207</v>
+        <v>-0.06440362645028737</v>
       </c>
       <c r="MO3">
-        <v>-0.04922353105910357</v>
+        <v>-0.056536940635</v>
       </c>
       <c r="MP3">
-        <v>-0.04724214075517449</v>
+        <v>-0.05446856093636911</v>
       </c>
       <c r="MQ3">
-        <v>-0.06325008978168337</v>
+        <v>-0.06947263355544789</v>
       </c>
       <c r="MR3">
-        <v>-0.06158142267262676</v>
+        <v>-0.06834278658876522</v>
       </c>
       <c r="MS3">
-        <v>-0.05761540139088083</v>
+        <v>-0.064403403402507</v>
       </c>
       <c r="MT3">
-        <v>-0.04922827945433845</v>
+        <v>-0.05654313921111892</v>
       </c>
       <c r="MU3">
-        <v>-0.04674656107186555</v>
+        <v>-0.05398204607009735</v>
       </c>
       <c r="MV3">
-        <v>-0.06326730154633808</v>
+        <v>-0.06948706786959492</v>
       </c>
       <c r="MW3">
-        <v>-0.06158170882574739</v>
+        <v>-0.0683452607451825</v>
       </c>
       <c r="MX3">
-        <v>-0.05761566448601935</v>
+        <v>-0.06440320802861517</v>
       </c>
       <c r="MY3">
-        <v>-0.04923162994558512</v>
+        <v>-0.05654751295966496</v>
       </c>
       <c r="MZ3">
-        <v>-0.04643603011858127</v>
+        <v>-0.05367719463425144</v>
       </c>
       <c r="NA3">
-        <v>-0.06328726827752433</v>
+        <v>-0.06950381257662511</v>
       </c>
       <c r="NB3">
-        <v>-0.06158185413596311</v>
+        <v>-0.06834651713712088</v>
       </c>
       <c r="NC3">
-        <v>-0.05761594402474599</v>
+        <v>-0.06440300044379246</v>
       </c>
       <c r="ND3">
-        <v>-0.04923505698281498</v>
+        <v>-0.05655198663384105</v>
       </c>
       <c r="NE3">
-        <v>-0.04595916921423545</v>
+        <v>-0.05320905460673699</v>
       </c>
       <c r="NF3">
-        <v>-0.06330921319156053</v>
+        <v>-0.0695222162396593</v>
       </c>
       <c r="NG3">
-        <v>-0.0615820677728797</v>
+        <v>-0.06834836430159644</v>
       </c>
       <c r="NH3">
-        <v>-0.05761634298659478</v>
+        <v>-0.06440270417571471</v>
       </c>
       <c r="NI3">
-        <v>-0.04923910064887849</v>
+        <v>-0.05655726526160243</v>
       </c>
       <c r="NJ3">
-        <v>-0.04548378610123772</v>
+        <v>-0.05274236442201628</v>
       </c>
       <c r="NK3">
-        <v>-0.06342885060816798</v>
+        <v>-0.06962254761419551</v>
       </c>
       <c r="NL3">
-        <v>-0.06158242589826091</v>
+        <v>-0.06835146075680586</v>
       </c>
       <c r="NM3">
-        <v>-0.05761682799825942</v>
+        <v>-0.06440234400738289</v>
       </c>
       <c r="NN3">
-        <v>-0.04924420145552928</v>
+        <v>-0.05656392389174813</v>
       </c>
       <c r="NO3">
-        <v>-0.0449503810820168</v>
+        <v>-0.05221871223187349</v>
       </c>
       <c r="NP3">
-        <v>-0.06426899040282893</v>
+        <v>-0.07023101499648023</v>
       </c>
       <c r="NQ3">
-        <v>-0.06345723144985072</v>
+        <v>-0.06969070558237375</v>
       </c>
       <c r="NR3">
-        <v>-0.06158402329432482</v>
+        <v>-0.06836527235038123</v>
       </c>
       <c r="NS3">
-        <v>-0.05761983426528225</v>
+        <v>-0.06440011156483727</v>
       </c>
       <c r="NT3">
-        <v>-0.04924876973440179</v>
+        <v>-0.05656988736027094</v>
       </c>
       <c r="NU3">
-        <v>-0.04456438360103754</v>
+        <v>-0.05183977164298143</v>
       </c>
       <c r="NV3">
-        <v>-0.06507377262802273</v>
+        <v>-0.0708138574480577</v>
       </c>
       <c r="NW3">
-        <v>-0.06363150169722294</v>
+        <v>-0.07010925115342743</v>
       </c>
       <c r="NX3">
-        <v>-0.06345723144988044</v>
+        <v>-0.06969070558232256</v>
       </c>
       <c r="NY3">
-        <v>-0.06158989530674595</v>
+        <v>-0.06841604429560093</v>
       </c>
       <c r="NZ3">
-        <v>-0.05763012102900247</v>
+        <v>-0.06439247269323843</v>
       </c>
       <c r="OA3">
-        <v>-0.0492523845052442</v>
+        <v>-0.05657460611432009</v>
       </c>
       <c r="OB3">
-        <v>-0.04410430253985387</v>
+        <v>-0.05138810109309196</v>
       </c>
       <c r="OC3">
-        <v>-0.06510960197179175</v>
+        <v>-0.07083980551674539</v>
       </c>
       <c r="OD3">
-        <v>-0.06369519659737069</v>
+        <v>-0.07026223909657339</v>
       </c>
       <c r="OE3">
-        <v>-0.06345723145003987</v>
+        <v>-0.06969070558204535</v>
       </c>
       <c r="OF3">
-        <v>-0.04925858833547873</v>
+        <v>-0.05658270465509315</v>
       </c>
       <c r="OG3">
-        <v>-0.043436717518286</v>
+        <v>-0.05073271832444733</v>
       </c>
       <c r="OH3">
-        <v>-0.06520834988676315</v>
+        <v>-0.07094177484606266</v>
       </c>
       <c r="OI3">
-        <v>-0.06570813867986673</v>
+        <v>-0.07125534056931949</v>
       </c>
       <c r="OJ3">
-        <v>-0.06370168000730267</v>
+        <v>-0.07027781186305292</v>
       </c>
       <c r="OK3">
-        <v>-0.06345723145005074</v>
+        <v>-0.0696907055820245</v>
       </c>
       <c r="OL3">
-        <v>-0.04928024537550203</v>
+        <v>-0.0566109760221957</v>
       </c>
       <c r="OM3">
-        <v>-0.04294177367036432</v>
+        <v>-0.05024681998677214</v>
       </c>
       <c r="ON3">
-        <v>-0.06521739796844792</v>
+        <v>-0.07095111810724378</v>
       </c>
       <c r="OO3">
-        <v>-0.06599692264422304</v>
+        <v>-0.07145582571801483</v>
       </c>
       <c r="OP3">
-        <v>-0.06370620459061495</v>
+        <v>-0.07028867968231212</v>
       </c>
       <c r="OQ3">
-        <v>-0.0634572314500562</v>
+        <v>-0.06969070558201591</v>
       </c>
       <c r="OR3">
-        <v>-0.04941265316285776</v>
+        <v>-0.05678382463523197</v>
       </c>
       <c r="OS3">
-        <v>-0.04246431190717732</v>
+        <v>-0.04977808328795412</v>
       </c>
       <c r="OT3">
-        <v>-0.06522254163276088</v>
+        <v>-0.07095642957611108</v>
       </c>
       <c r="OU3">
-        <v>-0.06686823285016213</v>
+        <v>-0.07206070932337019</v>
       </c>
       <c r="OV3">
-        <v>-0.06599692264434991</v>
+        <v>-0.07145582571810571</v>
       </c>
       <c r="OW3">
-        <v>-0.06371089166677989</v>
+        <v>-0.07029993783429955</v>
       </c>
       <c r="OX3">
-        <v>-0.0634572314500592</v>
+        <v>-0.06969070558201143</v>
       </c>
       <c r="OY3">
-        <v>-0.04199701226503113</v>
+        <v>-0.04931932210932416</v>
       </c>
       <c r="OZ3">
-        <v>-0.06522603431130916</v>
+        <v>-0.07096003619843808</v>
       </c>
       <c r="PA3">
-        <v>-0.06810943818473811</v>
+        <v>-0.07292234608008673</v>
       </c>
       <c r="PB3">
-        <v>-0.06599692264438149</v>
+        <v>-0.07145582571812824</v>
       </c>
       <c r="PC3">
-        <v>-0.063730574760842</v>
+        <v>-0.07034721613391508</v>
       </c>
       <c r="PD3">
-        <v>-0.06345723145006388</v>
+        <v>-0.06969070558200453</v>
       </c>
       <c r="PE3">
-        <v>-0.04143500278304856</v>
+        <v>-0.04876758044284419</v>
       </c>
       <c r="PF3">
-        <v>-0.06523172646489787</v>
+        <v>-0.07096591405102212</v>
       </c>
       <c r="PG3">
-        <v>-0.06836921113653921</v>
+        <v>-0.07310267335493535</v>
       </c>
       <c r="PH3">
-        <v>-0.06599692264440592</v>
+        <v>-0.07145582571814194</v>
       </c>
       <c r="PI3">
-        <v>-0.06373538093755692</v>
+        <v>-0.07035876054056185</v>
       </c>
       <c r="PJ3">
-        <v>-0.06345723145011686</v>
+        <v>-0.06969070558193308</v>
       </c>
       <c r="PK3">
-        <v>-0.04049371304802932</v>
+        <v>-0.04784348502358215</v>
       </c>
       <c r="PL3">
-        <v>-0.04143500278304856</v>
+        <v>-0.04876758044284419</v>
       </c>
       <c r="PM3">
-        <v>-0.06525064763772827</v>
+        <v>-0.07098545250571552</v>
       </c>
       <c r="PN3">
-        <v>-0.0684356081129911</v>
+        <v>-0.0731487640171789</v>
       </c>
       <c r="PO3">
-        <v>-0.06599692264443378</v>
+        <v>-0.07145582571815118</v>
       </c>
       <c r="PP3">
-        <v>-0.0637399655170114</v>
+        <v>-0.07036977270502749</v>
       </c>
       <c r="PQ3">
-        <v>-0.06345723145013477</v>
+        <v>-0.06969070558190756</v>
       </c>
       <c r="PR3">
-        <v>-0.03731856081101086</v>
+        <v>-0.04472630589827316</v>
       </c>
       <c r="PS3">
-        <v>-0.04049371304802932</v>
+        <v>-0.04784348502358215</v>
       </c>
       <c r="PT3">
-        <v>-0.06527171302711657</v>
+        <v>-0.07100720513607608</v>
       </c>
       <c r="PU3">
-        <v>-0.06847039285862833</v>
+        <v>-0.07317291042850764</v>
       </c>
       <c r="PV3">
-        <v>-0.06599692264446247</v>
+        <v>-0.07145582571815703</v>
       </c>
       <c r="PW3">
-        <v>-0.06374452517015609</v>
+        <v>-0.07038072502849445</v>
       </c>
       <c r="PX3">
-        <v>-0.06345723145014162</v>
+        <v>-0.06969070558189969</v>
       </c>
       <c r="PY3">
-        <v>-0.03282697230655539</v>
+        <v>-0.04031665630194348</v>
       </c>
       <c r="PZ3">
-        <v>-0.03731856081101086</v>
+        <v>-0.04472630589827316</v>
       </c>
       <c r="QA3">
-        <v>-0.06528356020842435</v>
+        <v>-0.07101943882490953</v>
       </c>
       <c r="QB3">
-        <v>-0.06849922917487514</v>
+        <v>-0.07319292761279575</v>
       </c>
       <c r="QC3">
-        <v>-0.06599692264448653</v>
+        <v>-0.07145582571815354</v>
       </c>
       <c r="QD3">
-        <v>-0.06374975569168201</v>
+        <v>-0.07039328882252358</v>
       </c>
       <c r="QE3">
-        <v>-0.06345723145015472</v>
+        <v>-0.06969070558188657</v>
       </c>
       <c r="QF3">
-        <v>-0.02960352118800055</v>
+        <v>-0.03715195909345562</v>
       </c>
       <c r="QG3">
-        <v>-0.03282697230655539</v>
+        <v>-0.04031665630194348</v>
       </c>
       <c r="QH3">
-        <v>-0.06529468943742883</v>
+        <v>-0.07103093114062109</v>
       </c>
       <c r="QI3">
-        <v>-0.06852259951733264</v>
+        <v>-0.07320915048805343</v>
       </c>
       <c r="QJ3">
-        <v>-0.06599692264451369</v>
+        <v>-0.07145582571815007</v>
       </c>
       <c r="QK3">
-        <v>-0.06376781908533927</v>
+        <v>-0.07043667769807677</v>
       </c>
       <c r="QL3">
-        <v>-0.06345723145016756</v>
+        <v>-0.06969070558187716</v>
       </c>
       <c r="QM3">
-        <v>-0.02862544771402515</v>
+        <v>-0.03619170460856745</v>
       </c>
       <c r="QN3">
-        <v>-0.02960352118800055</v>
+        <v>-0.03715195909345562</v>
       </c>
       <c r="QO3">
-        <v>-0.06530530769311892</v>
+        <v>-0.07104189581448829</v>
       </c>
       <c r="QP3">
-        <v>-0.06855832289025147</v>
+        <v>-0.07323394837606301</v>
       </c>
       <c r="QQ3">
-        <v>-0.06599692264453227</v>
+        <v>-0.07145582571814064</v>
       </c>
       <c r="QR3">
-        <v>-0.06385584767881626</v>
+        <v>-0.07064813249581008</v>
       </c>
       <c r="QS3">
-        <v>-0.06345723145018428</v>
+        <v>-0.06969070558186495</v>
       </c>
       <c r="QT3">
-        <v>-0.0256153232039807</v>
+        <v>-0.03336426468510057</v>
       </c>
       <c r="QU3">
-        <v>-0.02862544771402516</v>
+        <v>-0.03619170460856747</v>
       </c>
       <c r="QV3">
-        <v>-0.0287051033750653</v>
+        <v>-0.03616705449234556</v>
       </c>
       <c r="QW3">
-        <v>-0.06532274139656505</v>
+        <v>-0.07105989829230014</v>
       </c>
       <c r="QX3">
-        <v>-0.06859052716906389</v>
+        <v>-0.07325630340429008</v>
       </c>
       <c r="QY3">
-        <v>-0.06599692264454363</v>
+        <v>-0.07145582571813654</v>
       </c>
       <c r="QZ3">
-        <v>-0.06345723145019985</v>
+        <v>-0.06969070558185478</v>
       </c>
       <c r="RA3">
-        <v>-0.02227064009921703</v>
+        <v>-0.03022243658501314</v>
       </c>
       <c r="RB3">
-        <v>-0.02561532320398069</v>
+        <v>-0.03336426468510055</v>
       </c>
       <c r="RC3">
-        <v>-0.02561532320398069</v>
+        <v>-0.03336426468510056</v>
       </c>
       <c r="RD3">
-        <v>-0.02871673641435099</v>
+        <v>-0.03616345464833211</v>
       </c>
       <c r="RE3">
-        <v>-0.06533488438449474</v>
+        <v>-0.07107243744782478</v>
       </c>
       <c r="RF3">
-        <v>-0.06862117788216479</v>
+        <v>-0.07327757997736534</v>
       </c>
       <c r="RG3">
-        <v>-0.0659969226445508</v>
+        <v>-0.07145582571812942</v>
       </c>
       <c r="RH3">
-        <v>-0.06345723145027818</v>
+        <v>-0.0696907055818022</v>
       </c>
       <c r="RI3">
-        <v>-0.0210449069082514</v>
+        <v>-0.02907100879349968</v>
       </c>
       <c r="RJ3">
-        <v>-0.02227064009921703</v>
+        <v>-0.03022243658501314</v>
       </c>
       <c r="RK3">
-        <v>-0.02872307964049822</v>
+        <v>-0.03616149174753208</v>
       </c>
       <c r="RL3">
-        <v>-0.06534341635547095</v>
+        <v>-0.07108124777754589</v>
       </c>
       <c r="RM3">
-        <v>-0.06865570798178619</v>
+        <v>-0.07330154944337711</v>
       </c>
       <c r="RN3">
-        <v>-0.06599692264456214</v>
+        <v>-0.0714558257181203</v>
       </c>
       <c r="RO3">
-        <v>-0.06345723145028033</v>
+        <v>-0.06969070558179907</v>
       </c>
       <c r="RP3">
-        <v>-0.01846637846461562</v>
+        <v>-0.02663368782222071</v>
       </c>
       <c r="RQ3">
-        <v>-0.0210449069082514</v>
+        <v>-0.02907100879349968</v>
       </c>
       <c r="RR3">
-        <v>-0.02082917690737653</v>
+        <v>-0.02889654775530872</v>
       </c>
       <c r="RS3">
-        <v>-0.02872737669233303</v>
+        <v>-0.03616016203619927</v>
       </c>
       <c r="RT3">
-        <v>-0.06534749299390701</v>
+        <v>-0.0710854574182295</v>
       </c>
       <c r="RU3">
-        <v>-0.06869218312197564</v>
+        <v>-0.07332686904557797</v>
       </c>
       <c r="RV3">
-        <v>-0.06599692264458008</v>
+        <v>-0.07145582571811519</v>
       </c>
       <c r="RW3">
-        <v>-0.06345723145028156</v>
+        <v>-0.06969070558179709</v>
       </c>
       <c r="RX3">
-        <v>-0.01477046670508874</v>
+        <v>-0.02314004149577378</v>
       </c>
       <c r="RY3">
-        <v>-0.01846637846461562</v>
+        <v>-0.02663368782222071</v>
       </c>
       <c r="RZ3">
-        <v>-0.02083030349443668</v>
+        <v>-0.02889301438474942</v>
       </c>
       <c r="SA3">
-        <v>-0.0207357446275292</v>
+        <v>-0.02885230575497223</v>
       </c>
       <c r="SB3">
-        <v>-0.02873390365926344</v>
+        <v>-0.0361581422900631</v>
       </c>
       <c r="SC3">
-        <v>-0.06535007543651609</v>
+        <v>-0.07108812411437369</v>
       </c>
       <c r="SD3">
-        <v>-0.06877193591252614</v>
+        <v>-0.07338223015471572</v>
       </c>
       <c r="SE3">
-        <v>-0.06599692264460712</v>
+        <v>-0.07145582571811328</v>
       </c>
       <c r="SF3">
-        <v>-0.06345723145028172</v>
+        <v>-0.06969070558179501</v>
       </c>
       <c r="SG3">
-        <v>-0.01251481838617823</v>
+        <v>-0.02100776054394174</v>
       </c>
       <c r="SH3">
-        <v>-0.01477046670508874</v>
+        <v>-0.02314004149577378</v>
       </c>
       <c r="SI3">
-        <v>-0.02083077967680136</v>
+        <v>-0.02889152091276847</v>
       </c>
       <c r="SJ3">
-        <v>-0.02067595823158778</v>
+        <v>-0.02882399521287852</v>
       </c>
       <c r="SK3">
-        <v>-0.02874380902449323</v>
+        <v>-0.036155077125921</v>
       </c>
       <c r="SL3">
-        <v>-0.06535182148758821</v>
+        <v>-0.07108992713133176</v>
       </c>
       <c r="SM3">
-        <v>-0.07058107335810676</v>
+        <v>-0.07463801136543875</v>
       </c>
       <c r="SN3">
-        <v>-0.06599692264463033</v>
+        <v>-0.07145582571811218</v>
       </c>
       <c r="SO3">
-        <v>-0.06345723145028172</v>
+        <v>-0.06969070558179501</v>
       </c>
       <c r="SP3">
-        <v>-0.01212636070979531</v>
+        <v>-0.02064054274874147</v>
       </c>
       <c r="SQ3">
-        <v>-0.01251481838617823</v>
+        <v>-0.02100776054394174</v>
       </c>
       <c r="SR3">
-        <v>-0.02083105947242038</v>
+        <v>-0.02889064337791952</v>
       </c>
       <c r="SS3">
-        <v>-0.02875083658947679</v>
+        <v>-0.03615290249320445</v>
       </c>
       <c r="ST3">
-        <v>-0.06535425701991708</v>
+        <v>-0.07109244212432958</v>
       </c>
       <c r="SU3">
-        <v>-0.07061669621489675</v>
+        <v>-0.07468238713836901</v>
       </c>
       <c r="SV3">
-        <v>-0.07085100295933197</v>
+        <v>-0.07482110140418251</v>
       </c>
       <c r="SW3">
-        <v>-0.06599692264465111</v>
+        <v>-0.07145582571811382</v>
       </c>
       <c r="SX3">
-        <v>-0.01217059218923581</v>
+        <v>-0.02071169027813026</v>
       </c>
       <c r="SY3">
-        <v>-0.01212636070979532</v>
+        <v>-0.02064054274874148</v>
       </c>
       <c r="SZ3">
-        <v>-0.005284415213888635</v>
+        <v>-0.01388462673059797</v>
       </c>
       <c r="TA3">
-        <v>-0.02083131696872529</v>
+        <v>-0.02888983578176871</v>
       </c>
       <c r="TB3">
-        <v>-0.02875563792225784</v>
+        <v>-0.03615141675831639</v>
       </c>
       <c r="TC3">
-        <v>-0.06535611583917036</v>
+        <v>-0.07109436158870777</v>
       </c>
       <c r="TD3">
-        <v>-0.0706481113400113</v>
+        <v>-0.07472152144205006</v>
       </c>
       <c r="TE3">
-        <v>-0.07099662803216501</v>
+        <v>-0.07491987629247235</v>
       </c>
       <c r="TF3">
-        <v>-0.0659969226446694</v>
+        <v>-0.07145582571811529</v>
       </c>
       <c r="TG3">
-        <v>-0.01220315210664548</v>
+        <v>-0.02076406405180783</v>
       </c>
       <c r="TH3">
-        <v>-0.01217059218923581</v>
+        <v>-0.02071169027813026</v>
       </c>
       <c r="TI3">
-        <v>-0.001241140076304815</v>
+        <v>-0.009892057347636605</v>
       </c>
       <c r="TJ3">
-        <v>-0.0208315463763921</v>
+        <v>-0.02888911628148552</v>
       </c>
       <c r="TK3">
-        <v>-0.02875943192713386</v>
+        <v>-0.03615024273618442</v>
       </c>
       <c r="TL3">
-        <v>-0.0653693808299933</v>
+        <v>-0.07110805935957851</v>
       </c>
       <c r="TM3">
-        <v>-0.07101837662770373</v>
+        <v>-0.07493462792458401</v>
       </c>
       <c r="TN3">
-        <v>-0.06599692264468211</v>
+        <v>-0.07145582571811838</v>
       </c>
       <c r="TO3">
-        <v>-0.01224748285468114</v>
+        <v>-0.02083537198513511</v>
       </c>
       <c r="TP3">
-        <v>-0.01220315210664548</v>
+        <v>-0.02076406405180783</v>
       </c>
       <c r="TQ3">
-        <v>0.001962654178169683</v>
+        <v>-0.006728370575619536</v>
       </c>
       <c r="TR3">
-        <v>-0.02083178436089005</v>
+        <v>-0.02888836988168057</v>
       </c>
       <c r="TS3">
-        <v>-0.02877159657401955</v>
+        <v>-0.0361464785089138</v>
       </c>
       <c r="TT3">
-        <v>-0.06540032855709824</v>
+        <v>-0.07112315756433561</v>
       </c>
       <c r="TU3">
-        <v>-0.06541532413466017</v>
+        <v>-0.07120446346084346</v>
       </c>
       <c r="TV3">
-        <v>-0.07103497818821436</v>
+        <v>-0.07494588841790388</v>
       </c>
       <c r="TW3">
-        <v>-0.06599692264468961</v>
+        <v>-0.07145582571811755</v>
       </c>
       <c r="TX3">
-        <v>-0.01227885406119709</v>
+        <v>-0.02088583418682275</v>
       </c>
       <c r="TY3">
-        <v>-0.01224748285468114</v>
+        <v>-0.02083537198513511</v>
       </c>
       <c r="TZ3">
-        <v>0.003286517194642535</v>
+        <v>-0.005421062450710181</v>
       </c>
       <c r="UA3">
-        <v>-0.02083250279831991</v>
+        <v>-0.02888611662113923</v>
       </c>
       <c r="UB3">
-        <v>-0.02886999372546849</v>
+        <v>-0.03611603150802433</v>
       </c>
       <c r="UC3">
-        <v>-0.06543450242501488</v>
+        <v>-0.07113982955220682</v>
       </c>
       <c r="UD3">
-        <v>-0.0710505049823319</v>
+        <v>-0.0749564199123768</v>
       </c>
       <c r="UE3">
-        <v>-0.06599692264469921</v>
+        <v>-0.07145582571811607</v>
       </c>
       <c r="UF3">
-        <v>-0.01236658622093717</v>
+        <v>-0.02102695700122508</v>
       </c>
       <c r="UG3">
-        <v>-0.01227885406119709</v>
+        <v>-0.02088583418682275</v>
       </c>
       <c r="UH3">
-        <v>0.003359956231602834</v>
+        <v>-0.005350981414838398</v>
       </c>
       <c r="UI3">
-        <v>0.007800177143550808</v>
+        <v>-0.0009317007639272072</v>
       </c>
       <c r="UJ3">
-        <v>-0.02083322681162194</v>
+        <v>-0.02888384587588886</v>
       </c>
       <c r="UK3">
-        <v>-0.02887489395852717</v>
+        <v>-0.03611451527714989</v>
       </c>
       <c r="UL3">
-        <v>-0.06552713558701441</v>
+        <v>-0.07118502069315294</v>
       </c>
       <c r="UM3">
-        <v>-0.07106706242195826</v>
+        <v>-0.07496765046418197</v>
       </c>
       <c r="UN3">
-        <v>-0.06599692264470221</v>
+        <v>-0.07145582571810905</v>
       </c>
       <c r="UO3">
-        <v>-0.01243011398965833</v>
+        <v>-0.0211291465243507</v>
       </c>
       <c r="UP3">
-        <v>-0.01236658622093717</v>
+        <v>-0.02102695700122508</v>
       </c>
       <c r="UQ3">
-        <v>0.003386979598437997</v>
+        <v>-0.005325193664257031</v>
       </c>
       <c r="UR3">
-        <v>0.01121490615512904</v>
+        <v>0.00246468499840258</v>
       </c>
       <c r="US3">
-        <v>-0.02083999176304076</v>
+        <v>-0.0288626288998619</v>
       </c>
       <c r="UT3">
-        <v>-0.02887876042360553</v>
+        <v>-0.03611331891805553</v>
       </c>
       <c r="UU3">
-        <v>-0.0710817137790288</v>
+        <v>-0.07497758815502555</v>
       </c>
       <c r="UV3">
-        <v>-0.06599692264470222</v>
+        <v>-0.07145582571810906</v>
       </c>
       <c r="UW3">
-        <v>-0.0124421759375502</v>
+        <v>-0.02113925512581936</v>
       </c>
       <c r="UX3">
-        <v>-0.01243011398965833</v>
+        <v>-0.02112914652435071</v>
       </c>
       <c r="UY3">
-        <v>-0.01244508098434998</v>
+        <v>-0.0212232533382927</v>
       </c>
       <c r="UZ3">
-        <v>0.003427232939155572</v>
+        <v>-0.005286780839498208</v>
       </c>
       <c r="VA3">
-        <v>-0.0288831315781538</v>
+        <v>-0.03611196640160294</v>
       </c>
       <c r="VB3">
-        <v>-0.07109669955813688</v>
+        <v>-0.07498775267057202</v>
       </c>
       <c r="VC3">
-        <v>-0.01244503199005574</v>
+        <v>-0.02114164866036164</v>
       </c>
       <c r="VD3">
-        <v>-0.0124421759375502</v>
+        <v>-0.02113925512581936</v>
       </c>
       <c r="VE3">
-        <v>-0.01244697308269711</v>
+        <v>-0.02123515038045884</v>
       </c>
       <c r="VF3">
-        <v>0.003451454307584323</v>
+        <v>-0.005263666936315557</v>
       </c>
       <c r="VG3">
-        <v>-0.02888702205368933</v>
+        <v>-0.03611076261913748</v>
       </c>
       <c r="VH3">
-        <v>-0.07117404611974577</v>
+        <v>-0.07504021499431109</v>
       </c>
       <c r="VI3">
-        <v>-0.01252245915315938</v>
+        <v>-0.02120653693740751</v>
       </c>
       <c r="VJ3">
-        <v>-0.01244503199005573</v>
+        <v>-0.02114164866036163</v>
       </c>
       <c r="VK3">
-        <v>-0.01244503199002805</v>
+        <v>-0.02114164866034688</v>
       </c>
       <c r="VL3">
-        <v>-0.01244836932687574</v>
+        <v>-0.02124392965018058</v>
       </c>
       <c r="VM3">
-        <v>0.003480680587927551</v>
+        <v>-0.00523577694319136</v>
       </c>
       <c r="VN3">
-        <v>-0.02889150000210501</v>
+        <v>-0.03610937706555455</v>
       </c>
       <c r="VO3">
-        <v>-0.0712475271855635</v>
+        <v>-0.07507650081689819</v>
       </c>
       <c r="VP3">
-        <v>-0.07133014606328272</v>
+        <v>-0.07514802644848249</v>
       </c>
       <c r="VQ3">
-        <v>-0.01257672201289054</v>
+        <v>-0.02125201213163633</v>
       </c>
       <c r="VR3">
-        <v>-0.01252245915315938</v>
+        <v>-0.02120653693740751</v>
       </c>
       <c r="VS3">
-        <v>-0.01244503199001953</v>
+        <v>-0.02114164866034393</v>
       </c>
       <c r="VT3">
-        <v>-0.0124497278840607</v>
+        <v>-0.02125247198092907</v>
       </c>
       <c r="VU3">
-        <v>0.003506342514530551</v>
+        <v>-0.005211288319708685</v>
       </c>
       <c r="VV3">
-        <v>-0.02889609143537726</v>
+        <v>-0.03610795640166965</v>
       </c>
       <c r="VW3">
-        <v>-0.07125176176349285</v>
+        <v>-0.07507859188298988</v>
       </c>
       <c r="VX3">
-        <v>-0.07207616393120961</v>
+        <v>-0.07566325916098218</v>
       </c>
       <c r="VY3">
-        <v>-0.01264923760140505</v>
+        <v>-0.02128691149843105</v>
       </c>
       <c r="VZ3">
-        <v>-0.01258101801371932</v>
+        <v>-0.02125868207485326</v>
       </c>
       <c r="WA3">
-        <v>-0.01244503199001871</v>
+        <v>-0.02114164866033863</v>
       </c>
       <c r="WB3">
-        <v>-0.01246248972964189</v>
+        <v>-0.02133271723184415</v>
       </c>
       <c r="WC3">
-        <v>0.003674265869785595</v>
+        <v>-0.00505104235035269</v>
       </c>
       <c r="WD3">
-        <v>-0.02890161033668853</v>
+        <v>-0.03610624876929085</v>
       </c>
       <c r="WE3">
-        <v>-0.07125388852859084</v>
+        <v>-0.07507964209465079</v>
       </c>
       <c r="WF3">
-        <v>-0.07215120294273038</v>
+        <v>-0.07577073764794572</v>
       </c>
       <c r="WG3">
-        <v>-0.07292174441592704</v>
+        <v>-0.0762237928774625</v>
       </c>
       <c r="WH3">
-        <v>-0.01271390686950696</v>
+        <v>-0.02131803444770434</v>
       </c>
       <c r="WI3">
-        <v>-0.01264923760140505</v>
+        <v>-0.02128691149843105</v>
       </c>
       <c r="WJ3">
-        <v>-0.01264923760140505</v>
+        <v>-0.02128691149843105</v>
       </c>
       <c r="WK3">
-        <v>-0.0126723331357871</v>
+        <v>-0.02140057518778445</v>
       </c>
       <c r="WL3">
-        <v>-0.01258101801371932</v>
+        <v>-0.02125868207485326</v>
       </c>
       <c r="WM3">
-        <v>-0.01244503199001725</v>
+        <v>-0.02114164866033496</v>
       </c>
       <c r="WN3">
-        <v>-0.01246842923345659</v>
+        <v>-0.02137006509969399</v>
       </c>
       <c r="WO3">
-        <v>0.004912429713999936</v>
+        <v>-0.003869469136898902</v>
       </c>
       <c r="WP3">
-        <v>-0.02890507030404927</v>
+        <v>-0.03610517820540071</v>
       </c>
       <c r="WQ3">
-        <v>-0.07125567193805982</v>
+        <v>-0.07508052275447356</v>
       </c>
       <c r="WR3">
-        <v>-0.07219080229128787</v>
+        <v>-0.07582745649433378</v>
       </c>
       <c r="WS3">
-        <v>-0.07373179038258094</v>
+        <v>-0.07676075115471678</v>
       </c>
       <c r="WT3">
-        <v>-0.01277197132590085</v>
+        <v>-0.02134515163332712</v>
       </c>
       <c r="WU3">
-        <v>-0.01271390686950697</v>
+        <v>-0.02131803444770434</v>
       </c>
       <c r="WV3">
-        <v>-0.01271390686950695</v>
+        <v>-0.02131803444770431</v>
       </c>
       <c r="WW3">
-        <v>-0.01269382651013875</v>
+        <v>-0.0214339738755132</v>
       </c>
       <c r="WX3">
-        <v>-0.01244503199001469</v>
+        <v>-0.02114164866033281</v>
       </c>
       <c r="WY3">
-        <v>-0.01247121688947721</v>
+        <v>-0.02138759419094589</v>
       </c>
       <c r="WZ3">
-        <v>-0.02891994016183577</v>
+        <v>-0.03610057728174332</v>
       </c>
       <c r="XA3">
-        <v>-0.07125712624716415</v>
+        <v>-0.07508124090201246</v>
       </c>
       <c r="XB3">
-        <v>-0.07375145387741279</v>
+        <v>-0.07677993267530352</v>
       </c>
       <c r="XC3">
-        <v>-0.07394719118841855</v>
+        <v>-0.07689961119680175</v>
       </c>
       <c r="XD3">
-        <v>-0.01285107140500727</v>
+        <v>-0.02138209215077119</v>
       </c>
       <c r="XE3">
-        <v>-0.01244503199001143</v>
+        <v>-0.02114164866033211</v>
       </c>
       <c r="XF3">
-        <v>-0.01247307630114922</v>
+        <v>-0.02139928644397071</v>
       </c>
       <c r="XG3">
-        <v>-0.02898263117110077</v>
+        <v>-0.03608118033304251</v>
       </c>
       <c r="XH3">
-        <v>-0.07125940908954292</v>
+        <v>-0.07508236818432355</v>
       </c>
       <c r="XI3">
-        <v>-0.07375627544821375</v>
+        <v>-0.07678463606337003</v>
       </c>
       <c r="XJ3">
-        <v>-0.07399674963968567</v>
+        <v>-0.07693155929502257</v>
       </c>
       <c r="XK3">
-        <v>-0.0128742729832317</v>
+        <v>-0.02139292736428921</v>
       </c>
       <c r="XL3">
-        <v>-0.01244503199000925</v>
+        <v>-0.02114164866032874</v>
       </c>
       <c r="XM3">
-        <v>-0.01247591899854676</v>
+        <v>-0.02141716184306784</v>
       </c>
       <c r="XN3">
-        <v>-0.07126485266891053</v>
+        <v>-0.07508505625657655</v>
       </c>
       <c r="XO3">
-        <v>-0.07375958629364937</v>
+        <v>-0.07678786575569096</v>
       </c>
       <c r="XP3">
-        <v>-0.07402134309663541</v>
+        <v>-0.07694741356002394</v>
       </c>
       <c r="XQ3">
-        <v>-0.01295106795913812</v>
+        <v>-0.02142879037799417</v>
       </c>
       <c r="XR3">
-        <v>-0.01244503199000641</v>
+        <v>-0.02114164866032634</v>
       </c>
       <c r="XS3">
-        <v>-0.01248147076404283</v>
+        <v>-0.0214520727092842</v>
       </c>
       <c r="XT3">
-        <v>-0.07126861875234362</v>
+        <v>-0.07508691596926241</v>
       </c>
       <c r="XU3">
-        <v>-0.07376417585046822</v>
+        <v>-0.07679234281632166</v>
       </c>
       <c r="XV3">
-        <v>-0.07404836952056514</v>
+        <v>-0.07696483622541159</v>
       </c>
       <c r="XW3">
-        <v>-0.01244503199000537</v>
+        <v>-0.02114164866032573</v>
       </c>
       <c r="XX3">
-        <v>-0.01248300541706389</v>
+        <v>-0.02146172306719794</v>
       </c>
       <c r="XY3">
-        <v>-0.07127340731407605</v>
+        <v>-0.07508928058501417</v>
       </c>
       <c r="XZ3">
-        <v>-0.07377505909934343</v>
+        <v>-0.07680295930126128</v>
       </c>
       <c r="YA3">
-        <v>-0.07407955416791201</v>
+        <v>-0.07698493947471784</v>
       </c>
       <c r="YB3">
-        <v>-0.0124450319900061</v>
+        <v>-0.0211416486603276</v>
       </c>
       <c r="YC3">
-        <v>-0.01248345095165598</v>
+        <v>-0.02146452472886672</v>
       </c>
       <c r="YD3">
-        <v>-0.07127631632973631</v>
+        <v>-0.07509071707023049</v>
       </c>
       <c r="YE3">
-        <v>-0.07378333219766611</v>
+        <v>-0.0768110296132937</v>
       </c>
       <c r="YF3">
-        <v>-0.07411107991748402</v>
+        <v>-0.07700526258657053</v>
       </c>
       <c r="YG3">
-        <v>-0.01244503199000549</v>
+        <v>-0.02114164866032998</v>
       </c>
       <c r="YH3">
-        <v>-0.01248383922406321</v>
+        <v>-0.02146531427674329</v>
       </c>
       <c r="YI3">
-        <v>-0.01248344145910461</v>
+        <v>-0.02147324010475196</v>
       </c>
       <c r="YJ3">
-        <v>-0.0712789425538104</v>
+        <v>-0.07509201391084239</v>
       </c>
       <c r="YK3">
-        <v>-0.07378913980568821</v>
+        <v>-0.07681669486751776</v>
       </c>
       <c r="YL3">
-        <v>-0.07414603051216621</v>
+        <v>-0.07702779349394615</v>
       </c>
       <c r="YM3">
-        <v>-0.01244503199000009</v>
+        <v>-0.02114164866032855</v>
       </c>
       <c r="YN3">
-        <v>-0.01248420261409726</v>
+        <v>-0.0214660532267066</v>
       </c>
       <c r="YO3">
-        <v>-0.01248342893306283</v>
+        <v>-0.02148474066877617</v>
       </c>
       <c r="YP3">
-        <v>-0.07128337178076991</v>
+        <v>-0.07509420108016364</v>
       </c>
       <c r="YQ3">
-        <v>-0.07379522379966987</v>
+        <v>-0.07682262973264524</v>
       </c>
       <c r="YR3">
-        <v>-0.07419685642621317</v>
+        <v>-0.07706055836336806</v>
       </c>
       <c r="YS3">
-        <v>-0.01244503198999496</v>
+        <v>-0.02114164866032528</v>
       </c>
       <c r="YT3">
-        <v>-0.01248457695278858</v>
+        <v>-0.02146681444078464</v>
       </c>
       <c r="YU3">
-        <v>-0.01248337689409226</v>
+        <v>-0.02153251997824819</v>
       </c>
       <c r="YV3">
-        <v>-0.07128772631883931</v>
+        <v>-0.07509635136564224</v>
       </c>
       <c r="YW3">
-        <v>-0.07380021883155198</v>
+        <v>-0.07682750232765241</v>
       </c>
       <c r="YX3">
-        <v>-0.07409810531792645</v>
+        <v>-0.07695737558156786</v>
       </c>
       <c r="YY3">
-        <v>-0.07435089132741392</v>
+        <v>-0.07717115724981437</v>
       </c>
       <c r="YZ3">
-        <v>-0.01244503198999327</v>
+        <v>-0.02114164866032177</v>
       </c>
       <c r="ZA3">
-        <v>-0.01248728350757425</v>
+        <v>-0.02147231819756093</v>
       </c>
       <c r="ZB3">
-        <v>-0.01248335479438871</v>
+        <v>-0.02155281101997811</v>
       </c>
       <c r="ZC3">
-        <v>-0.07128978665193733</v>
+        <v>-0.07509736876427166</v>
       </c>
       <c r="ZD3">
-        <v>-0.07380848925447016</v>
+        <v>-0.07683557002759604</v>
       </c>
       <c r="ZE3">
-        <v>-0.07403880471617443</v>
+        <v>-0.0768954138350857</v>
       </c>
       <c r="ZF3">
-        <v>-0.07532635506379155</v>
+        <v>-0.07787153713996776</v>
       </c>
       <c r="ZG3">
-        <v>-0.01244503198999327</v>
+        <v>-0.02114164866032177</v>
       </c>
       <c r="ZH3">
-        <v>-0.01250699304404799</v>
+        <v>-0.02151239758871803</v>
       </c>
       <c r="ZI3">
-        <v>-0.0712920496506092</v>
+        <v>-0.07509848623920858</v>
       </c>
       <c r="ZJ3">
-        <v>-0.07383521702469664</v>
+        <v>-0.07686164264688963</v>
       </c>
       <c r="ZK3">
-        <v>-0.07398379444463873</v>
+        <v>-0.07683793501693564</v>
       </c>
       <c r="ZL3">
-        <v>-0.07602467427938826</v>
+        <v>-0.07837291260168382</v>
       </c>
       <c r="ZM3">
-        <v>-0.07129422164705791</v>
+        <v>-0.07509955877644925</v>
       </c>
       <c r="ZN3">
-        <v>-0.07389767104590443</v>
+        <v>-0.07692256576517159</v>
       </c>
       <c r="ZO3">
-        <v>-0.07393011875686366</v>
+        <v>-0.07678185073352808</v>
       </c>
       <c r="ZP3">
-        <v>-0.07605712604809961</v>
+        <v>-0.07843979953588173</v>
       </c>
       <c r="ZQ3">
-        <v>-0.07798797913631164</v>
+        <v>-0.07973562480958782</v>
       </c>
       <c r="ZR3">
-        <v>-0.07129684105962854</v>
+        <v>-0.07510085224816759</v>
       </c>
       <c r="ZS3">
-        <v>-0.07388985816416248</v>
+        <v>-0.07673978356288881</v>
       </c>
       <c r="ZT3">
-        <v>-0.07605709389512069</v>
+        <v>-0.07844605827231382</v>
       </c>
       <c r="ZU3">
-        <v>-0.0760656873387727</v>
+        <v>-0.07843978776497663</v>
       </c>
       <c r="ZV3">
-        <v>-0.0780639997504663</v>
+        <v>-0.07977339370724308</v>
       </c>
       <c r="ZW3">
-        <v>-0.07838204596091344</v>
+        <v>-0.08001198454455036</v>
       </c>
       <c r="ZX3">
-        <v>-0.07130101936102702</v>
+        <v>-0.07510291550101648</v>
       </c>
       <c r="ZY3">
-        <v>-0.07382590115845333</v>
+        <v>-0.07667295674247515</v>
       </c>
       <c r="ZZ3">
-        <v>-0.07605708383425246</v>
+        <v>-0.07844801667360347</v>
       </c>
       <c r="AAA3">
-        <v>-0.0760831281371805</v>
+        <v>-0.07843976378579247</v>
       </c>
       <c r="AAB3">
-        <v>-0.07810804171994064</v>
+        <v>-0.07979527453182754</v>
       </c>
       <c r="AAC3">
-        <v>-0.07879593944633058</v>
+        <v>-0.0802935390170674</v>
       </c>
       <c r="AAD3">
-        <v>-0.07131245494869895</v>
+        <v>-0.07510856240488294</v>
       </c>
       <c r="AAE3">
-        <v>-0.07371806604353556</v>
+        <v>-0.07656028315672468</v>
       </c>
       <c r="AAF3">
-        <v>-0.07605707736540615</v>
+        <v>-0.07844927586985148</v>
       </c>
       <c r="AAG3">
-        <v>-0.07988793378255316</v>
+        <v>-0.08103633806809282</v>
       </c>
       <c r="AAH3">
-        <v>-0.07879593944631713</v>
+        <v>-0.0802935390170566</v>
       </c>
       <c r="AAI3">
-        <v>-0.07132767371054895</v>
+        <v>-0.07511607742056998</v>
       </c>
       <c r="AAJ3">
-        <v>-0.07291001894112255</v>
+        <v>-0.07571598758861939</v>
       </c>
       <c r="AAK3">
-        <v>-0.07605707346357882</v>
+        <v>-0.07845003538201448</v>
       </c>
       <c r="AAL3">
-        <v>-0.0812071252832286</v>
+        <v>-0.08197170388961984</v>
       </c>
       <c r="AAM3">
-        <v>-0.07980192716314101</v>
+        <v>-0.08093172947171186</v>
       </c>
       <c r="AAN3">
-        <v>-0.07879593944630429</v>
+        <v>-0.08029353901704417</v>
       </c>
       <c r="AAO3">
-        <v>-0.07132912325370086</v>
+        <v>-0.07511679320275219</v>
       </c>
       <c r="AAP3">
-        <v>-0.07224706139039236</v>
+        <v>-0.07502330064097877</v>
       </c>
       <c r="AAQ3">
-        <v>-0.07605706951995264</v>
+        <v>-0.07845080303051509</v>
       </c>
       <c r="AAR3">
-        <v>-0.08256911264122301</v>
+        <v>-0.0829373314665881</v>
       </c>
       <c r="AAS3">
-        <v>-0.07979271983662195</v>
+        <v>-0.0809205307875118</v>
       </c>
       <c r="AAT3">
-        <v>-0.07879593944629111</v>
+        <v>-0.08029353901703422</v>
       </c>
       <c r="AAU3">
-        <v>-0.07133026963554905</v>
+        <v>-0.07511735928417831</v>
       </c>
       <c r="AAV3">
-        <v>-0.07203700229723592</v>
+        <v>-0.07480382370819984</v>
       </c>
       <c r="AAW3">
-        <v>-0.07605706599746599</v>
+        <v>-0.07845148870236769</v>
       </c>
       <c r="AAX3">
-        <v>-0.08309674841143919</v>
+        <v>-0.08328774475129756</v>
       </c>
       <c r="AAY3">
-        <v>-0.08271983294864177</v>
+        <v>-0.08312386481651592</v>
       </c>
       <c r="AAZ3">
-        <v>-0.07978920434585771</v>
+        <v>-0.08091625497020258</v>
       </c>
       <c r="ABA3">
-        <v>-0.07879593944628269</v>
+        <v>-0.08029353901702432</v>
       </c>
       <c r="ABB3">
-        <v>-0.07133138304766623</v>
+        <v>-0.07511790908506298</v>
       </c>
       <c r="ABC3">
-        <v>-0.07184576568600644</v>
+        <v>-0.07460401397102227</v>
       </c>
       <c r="ABD3">
-        <v>-0.07605706202884716</v>
+        <v>-0.07845226121658368</v>
       </c>
       <c r="ABE3">
-        <v>-0.0838138309987539</v>
+        <v>-0.08376395161947549</v>
       </c>
       <c r="ABF3">
-        <v>-0.08274005178440348</v>
+        <v>-0.08314888813398331</v>
       </c>
       <c r="ABG3">
-        <v>-0.07978548564881699</v>
+        <v>-0.08091173199899966</v>
       </c>
       <c r="ABH3">
-        <v>-0.07879593944627815</v>
+        <v>-0.0802935390170165</v>
       </c>
       <c r="ABI3">
-        <v>-0.07133257563268994</v>
+        <v>-0.07511849798122867</v>
       </c>
       <c r="ABJ3">
-        <v>-0.07174160612962446</v>
+        <v>-0.07449518527747108</v>
       </c>
       <c r="ABK3">
-        <v>-0.07605705884918226</v>
+        <v>-0.07845288015680138</v>
       </c>
       <c r="ABL3">
-        <v>-0.08465354796275265</v>
+        <v>-0.08432156678058655</v>
       </c>
       <c r="ABM3">
-        <v>-0.08275067436654644</v>
+        <v>-0.08316203491912132</v>
       </c>
       <c r="ABN3">
-        <v>-0.0797823994501366</v>
+        <v>-0.08090797832320576</v>
       </c>
       <c r="ABO3">
-        <v>-0.07879593944627362</v>
+        <v>-0.08029353901700874</v>
       </c>
       <c r="ABP3">
-        <v>-0.07133367826818847</v>
+        <v>-0.07511904246034896</v>
       </c>
       <c r="ABQ3">
-        <v>-0.07165841745372929</v>
+        <v>-0.07440826768832012</v>
       </c>
       <c r="ABR3">
-        <v>-0.07605705503517317</v>
+        <v>-0.07845362257627253</v>
       </c>
       <c r="ABS3">
-        <v>-0.0853279301491783</v>
+        <v>-0.08476936626260866</v>
       </c>
       <c r="ABT3">
-        <v>-0.08279593850673116</v>
+        <v>-0.08319145122343835</v>
       </c>
       <c r="ABU3">
-        <v>-0.08275116465727658</v>
+        <v>-0.08316350997298122</v>
       </c>
       <c r="ABV3">
-        <v>-0.07977874462885143</v>
+        <v>-0.08090353304568337</v>
       </c>
       <c r="ABW3">
-        <v>-0.07879593944627028</v>
+        <v>-0.08029353901700551</v>
       </c>
       <c r="ABX3">
-        <v>-0.07133471738610948</v>
+        <v>-0.07511955557449396</v>
       </c>
       <c r="ABY3">
-        <v>-0.07158748050208627</v>
+        <v>-0.07433415112124783</v>
       </c>
       <c r="ABZ3">
-        <v>-0.07605705092512083</v>
+        <v>-0.0784544226223358</v>
       </c>
       <c r="ACA3">
-        <v>-0.08556245039820912</v>
+        <v>-0.08482943465382367</v>
       </c>
       <c r="ACB3">
-        <v>-0.08539965750250811</v>
+        <v>-0.08524762993083593</v>
       </c>
       <c r="ACC3">
-        <v>-0.08283273333509238</v>
+        <v>-0.08321536332634147</v>
       </c>
       <c r="ACD3">
-        <v>-0.08275151920801208</v>
+        <v>-0.08316457664954821</v>
       </c>
       <c r="ACE3">
-        <v>-0.07977518028623951</v>
+        <v>-0.08089919781689622</v>
       </c>
       <c r="ACF3">
-        <v>-0.07879593944626617</v>
+        <v>-0.08029353901700241</v>
       </c>
       <c r="ACG3">
-        <v>-0.07133616260113483</v>
+        <v>-0.07512026921829189</v>
       </c>
       <c r="ACH3">
-        <v>-0.07150423471473041</v>
+        <v>-0.07424717413553208</v>
       </c>
       <c r="ACI3">
-        <v>-0.07605704342654618</v>
+        <v>-0.07845588226540877</v>
       </c>
       <c r="ACJ3">
-        <v>-0.08588580756892315</v>
+        <v>-0.08491225336510175</v>
       </c>
       <c r="ACK3">
-        <v>-0.08545961396386689</v>
+        <v>-0.08564747570357249</v>
       </c>
       <c r="ACL3">
-        <v>-0.08275181841726635</v>
+        <v>-0.08316547682987101</v>
       </c>
       <c r="ACM3">
-        <v>-0.07977028007279942</v>
+        <v>-0.08089323780132081</v>
       </c>
       <c r="ACN3">
-        <v>-0.07879593944626261</v>
+        <v>-0.08029353901700098</v>
       </c>
       <c r="ACO3">
-        <v>-0.07133793365429007</v>
+        <v>-0.07512114375987063</v>
       </c>
       <c r="ACP3">
-        <v>-0.07142816898957627</v>
+        <v>-0.07416769916274514</v>
       </c>
       <c r="ACQ3">
-        <v>-0.07605698732550402</v>
+        <v>-0.07846680270484034</v>
       </c>
       <c r="ACR3">
-        <v>-0.08668138435391709</v>
+        <v>-0.08511599913453562</v>
       </c>
       <c r="ACS3">
-        <v>-0.08547414253811343</v>
+        <v>-0.08567725298881529</v>
       </c>
       <c r="ACT3">
-        <v>-0.08546066693858775</v>
+        <v>-0.08565692888536863</v>
       </c>
       <c r="ACU3">
-        <v>-0.08275232381640274</v>
+        <v>-0.08316699733940643</v>
       </c>
       <c r="ACV3">
-        <v>-0.07976353902539642</v>
+        <v>-0.08088503882694881</v>
       </c>
       <c r="ACW3">
-        <v>-0.0787959394462638</v>
+        <v>-0.0802935390169995</v>
       </c>
       <c r="ACX3">
-        <v>-0.07134632800648982</v>
+        <v>-0.07512528886493576</v>
       </c>
       <c r="ACY3">
-        <v>-0.07131016069834567</v>
+        <v>-0.0740444020133995</v>
       </c>
       <c r="ACZ3">
-        <v>-0.07605681540418185</v>
+        <v>-0.0785002686691159</v>
       </c>
       <c r="ADA3">
-        <v>-0.08732632364931374</v>
+        <v>-0.08528114759143142</v>
       </c>
       <c r="ADB3">
-        <v>-0.08548837907656125</v>
+        <v>-0.08570643192801536</v>
       </c>
       <c r="ADC3">
-        <v>-0.08546167371797304</v>
+        <v>-0.08566596737797449</v>
       </c>
       <c r="ADD3">
-        <v>-0.08275303156826408</v>
+        <v>-0.08316912663479778</v>
       </c>
       <c r="ADE3">
-        <v>-0.07975640507523708</v>
+        <v>-0.0808763619803225</v>
       </c>
       <c r="ADF3">
-        <v>-0.07879593944626608</v>
+        <v>-0.08029353901700095</v>
       </c>
       <c r="ADG3">
-        <v>-0.07141810343405876</v>
+        <v>-0.07516073102034233</v>
       </c>
       <c r="ADH3">
-        <v>-0.07107190855951291</v>
+        <v>-0.07379547287503933</v>
       </c>
       <c r="ADI3">
-        <v>-0.08783033068017695</v>
+        <v>-0.08541019573090211</v>
       </c>
       <c r="ADJ3">
-        <v>-0.0854627590792665</v>
+        <v>-0.08567571138693654</v>
       </c>
       <c r="ADK3">
-        <v>-0.08275355673685426</v>
+        <v>-0.08317070662314278</v>
       </c>
       <c r="ADL3">
-        <v>-0.07975166617988846</v>
+        <v>-0.08087059818283918</v>
       </c>
       <c r="ADM3">
-        <v>-0.07879593944626823</v>
+        <v>-0.08029353901700317</v>
       </c>
       <c r="ADN3">
-        <v>-0.07099711416107057</v>
+        <v>-0.07371762578089724</v>
       </c>
       <c r="ADO3">
-        <v>-0.07109351411340011</v>
+        <v>-0.07381626475427583</v>
       </c>
       <c r="ADP3">
-        <v>-0.08828590869483692</v>
+        <v>-0.08552683480489005</v>
       </c>
       <c r="ADQ3">
-        <v>-0.08546372822443861</v>
+        <v>-0.08568441207913645</v>
       </c>
       <c r="ADR3">
-        <v>-0.08275442670076683</v>
+        <v>-0.08317332394212987</v>
       </c>
       <c r="ADS3">
-        <v>-0.07974684311860664</v>
+        <v>-0.08086473201925108</v>
       </c>
       <c r="ADT3">
-        <v>-0.07879593944627195</v>
+        <v>-0.08029353901700381</v>
       </c>
       <c r="ADU3">
-        <v>-0.07093188601830128</v>
+        <v>-0.0736497354731073</v>
       </c>
       <c r="ADV3">
-        <v>-0.071128086825516</v>
+        <v>-0.07384953542679445</v>
       </c>
       <c r="ADW3">
-        <v>-0.08829412825926528</v>
+        <v>-0.08552277486692005</v>
       </c>
       <c r="ADX3">
-        <v>-0.08856257254483388</v>
+        <v>-0.08563148939813234</v>
       </c>
       <c r="ADY3">
-        <v>-0.08546479848427653</v>
+        <v>-0.08569402058385758</v>
       </c>
       <c r="ADZ3">
-        <v>-0.082760465146378</v>
+        <v>-0.08319149088921299</v>
       </c>
       <c r="AEA3">
-        <v>-0.07974453700364795</v>
+        <v>-0.08086192715278902</v>
       </c>
       <c r="AEB3">
-        <v>-0.07879593944627428</v>
+        <v>-0.0802935390170052</v>
       </c>
       <c r="AEC3">
-        <v>-0.07087793911362646</v>
+        <v>-0.07359358688859609</v>
       </c>
       <c r="AED3">
-        <v>-0.07115762649079377</v>
+        <v>-0.07387796258589925</v>
       </c>
       <c r="AEE3">
-        <v>-0.08830236948002482</v>
+        <v>-0.08551870425496134</v>
       </c>
       <c r="AEF3">
-        <v>-0.08886999814276687</v>
+        <v>-0.08574769149005468</v>
       </c>
       <c r="AEG3">
-        <v>-0.08856257254483388</v>
+        <v>-0.08563148939813234</v>
       </c>
       <c r="AEH3">
-        <v>-0.08546548851624487</v>
+        <v>-0.08570021552495687</v>
       </c>
       <c r="AEI3">
-        <v>-0.08277380338755339</v>
+        <v>-0.08323161997004444</v>
       </c>
       <c r="AEJ3">
-        <v>-0.07974086884536333</v>
+        <v>-0.08085746567047153</v>
       </c>
       <c r="AEK3">
-        <v>-0.07879593944627752</v>
+        <v>-0.08029353901700111</v>
       </c>
       <c r="AEL3">
-        <v>-0.07083598721660139</v>
+        <v>-0.07354992289081402</v>
       </c>
       <c r="AEM3">
-        <v>-0.07117434505533077</v>
+        <v>-0.07389405149891193</v>
       </c>
       <c r="AEN3">
-        <v>-0.08831062675900224</v>
+        <v>-0.08551462573426535</v>
       </c>
       <c r="AEO3">
-        <v>-0.08912778007723339</v>
+        <v>-0.08584512531071772</v>
       </c>
       <c r="AEP3">
-        <v>-0.08886999814276687</v>
+        <v>-0.08574769149005468</v>
       </c>
       <c r="AEQ3">
-        <v>-0.08546654835863182</v>
+        <v>-0.08570973056535822</v>
       </c>
       <c r="AER3">
-        <v>-0.07973742525614069</v>
+        <v>-0.08085327732693824</v>
       </c>
       <c r="AES3">
-        <v>-0.07879593944627911</v>
+        <v>-0.08029353901700376</v>
       </c>
       <c r="AET3">
-        <v>-0.07079331939421239</v>
+        <v>-0.07350551378509676</v>
       </c>
       <c r="AEU3">
-        <v>-0.08831883411385491</v>
+        <v>-0.08551057189536986</v>
       </c>
       <c r="AEV3">
-        <v>-0.08940490535697643</v>
+        <v>-0.08594986653045737</v>
       </c>
       <c r="AEW3">
-        <v>-0.08912778007723339</v>
+        <v>-0.08584512531071774</v>
       </c>
       <c r="AEX3">
-        <v>-0.08547526584979798</v>
+        <v>-0.08578799574625398</v>
       </c>
       <c r="AEY3">
-        <v>-0.07973250493421433</v>
+        <v>-0.08084729287621846</v>
       </c>
       <c r="AEZ3">
-        <v>-0.07879593944627911</v>
+        <v>-0.08029353901700376</v>
       </c>
       <c r="AFA3">
-        <v>-0.07075629119077739</v>
+        <v>-0.0734669744811184</v>
       </c>
       <c r="AFB3">
-        <v>-0.08832707272301624</v>
+        <v>-0.08550650264193144</v>
       </c>
       <c r="AFC3">
-        <v>-0.08963244760845733</v>
+        <v>-0.08603586459032338</v>
       </c>
       <c r="AFD3">
-        <v>-0.08940490535697643</v>
+        <v>-0.08594986653045737</v>
       </c>
       <c r="AFE3">
-        <v>-0.08550531052963742</v>
+        <v>-0.08605775433699185</v>
       </c>
       <c r="AFF3">
-        <v>-0.07968056719871945</v>
+        <v>-0.08078412263053227</v>
       </c>
       <c r="AFG3">
-        <v>-0.07072969690194651</v>
+        <v>-0.07343929491048566</v>
       </c>
       <c r="AFH3">
-        <v>-0.08833530579593109</v>
+        <v>-0.08550243614582285</v>
       </c>
       <c r="AFI3">
-        <v>-0.089876751889295</v>
+        <v>-0.08612819478847079</v>
       </c>
       <c r="AFJ3">
-        <v>-0.08963244760845732</v>
+        <v>-0.08603586459032334</v>
       </c>
       <c r="AFK3">
-        <v>-0.07965979321104091</v>
+        <v>-0.08075885596890357</v>
       </c>
       <c r="AFL3">
-        <v>-0.07069882081180141</v>
+        <v>-0.07340715882048611</v>
       </c>
       <c r="AFM3">
-        <v>-0.08834354412965673</v>
+        <v>-0.085498367074141</v>
       </c>
       <c r="AFN3">
-        <v>-0.09042054842385205</v>
+        <v>-0.08633299007714725</v>
       </c>
       <c r="AFO3">
-        <v>-0.08987675188928852</v>
+        <v>-0.08612819478845837</v>
       </c>
       <c r="AFP3">
-        <v>-0.089876751889295</v>
+        <v>-0.08612819478847079</v>
       </c>
       <c r="AFQ3">
-        <v>-0.07964924417249473</v>
+        <v>-0.08074602556874669</v>
       </c>
       <c r="AFR3">
-        <v>-0.07065230542055051</v>
+        <v>-0.07335874525152784</v>
       </c>
       <c r="AFS3">
-        <v>-0.08834756554380344</v>
+        <v>-0.0854963808285517</v>
       </c>
       <c r="AFT3">
-        <v>-0.09050012029862693</v>
+        <v>-0.08636295406050315</v>
       </c>
       <c r="AFU3">
-        <v>-0.089876751889282</v>
+        <v>-0.08612819478844401</v>
       </c>
       <c r="AFV3">
-        <v>-0.08987675188928852</v>
+        <v>-0.08612819478845837</v>
       </c>
       <c r="AFW3">
-        <v>-0.0796469098705634</v>
+        <v>-0.08074318644661353</v>
       </c>
       <c r="AFX3">
-        <v>-0.07057630827563979</v>
+        <v>-0.07327964694218091</v>
       </c>
       <c r="AFY3">
-        <v>-0.08843795131931693</v>
+        <v>-0.08545173917721932</v>
       </c>
       <c r="AFZ3">
-        <v>-0.09072430986606501</v>
+        <v>-0.08644737187923693</v>
       </c>
       <c r="AGA3">
-        <v>-0.08987675188928096</v>
+        <v>-0.08612819478842752</v>
       </c>
       <c r="AGB3">
-        <v>-0.089876751889282</v>
+        <v>-0.08612819478844401</v>
       </c>
       <c r="AGC3">
-        <v>-0.07964507149230786</v>
+        <v>-0.08074095049793555</v>
       </c>
       <c r="AGD3">
-        <v>-0.06995962522527067</v>
+        <v>-0.07261728530075939</v>
       </c>
       <c r="AGE3">
-        <v>-0.0705945250103177</v>
+        <v>-0.07335325209955611</v>
       </c>
       <c r="AGF3">
-        <v>-0.08849673150218304</v>
+        <v>-0.08542270904563928</v>
       </c>
       <c r="AGG3">
-        <v>-0.09098759790892907</v>
+        <v>-0.08654650431913721</v>
       </c>
       <c r="AGH3">
-        <v>-0.08987675188927928</v>
+        <v>-0.0861281947884142</v>
       </c>
       <c r="AGI3">
-        <v>-0.08987675188928096</v>
+        <v>-0.08612819478842752</v>
       </c>
       <c r="AGJ3">
-        <v>-0.07964310178938107</v>
+        <v>-0.08073855482456858</v>
       </c>
       <c r="AGK3">
-        <v>-0.08854814327268032</v>
+        <v>-0.08539731895139337</v>
       </c>
       <c r="AGL3">
-        <v>-0.09102175468564123</v>
+        <v>-0.08655936431275335</v>
       </c>
       <c r="AGM3">
-        <v>-0.08987675188927781</v>
+        <v>-0.08612819478840784</v>
       </c>
       <c r="AGN3">
-        <v>-0.08987675188927928</v>
+        <v>-0.0861281947884142</v>
       </c>
       <c r="AGO3">
-        <v>-0.07964152588240345</v>
+        <v>-0.08073663811029523</v>
       </c>
       <c r="AGP3">
-        <v>-0.08860207345153998</v>
+        <v>-0.08537068607869575</v>
       </c>
       <c r="AGQ3">
-        <v>-0.09105717673559324</v>
+        <v>-0.08656514032584665</v>
       </c>
       <c r="AGR3">
-        <v>-0.09103846728914139</v>
+        <v>-0.08658247720504691</v>
       </c>
       <c r="AGS3">
-        <v>-0.08987675188927774</v>
+        <v>-0.08612819478840779</v>
       </c>
       <c r="AGT3">
-        <v>-0.08987675188927778</v>
+        <v>-0.08612819478840782</v>
       </c>
       <c r="AGU3">
-        <v>-0.07963999574072639</v>
+        <v>-0.08073477705886163</v>
       </c>
       <c r="AGV3">
-        <v>-0.08869416453220788</v>
+        <v>-0.08532521009542041</v>
       </c>
       <c r="AGW3">
-        <v>-0.09108995428447748</v>
+        <v>-0.08657048504087227</v>
       </c>
       <c r="AGX3">
-        <v>-0.09107757984652461</v>
+        <v>-0.08663656867643181</v>
       </c>
       <c r="AGY3">
-        <v>-0.08987675188927774</v>
+        <v>-0.08612819478840779</v>
       </c>
       <c r="AGZ3">
-        <v>-0.08987675188927773</v>
+        <v>-0.08612819478840775</v>
       </c>
       <c r="AHA3">
-        <v>-0.07963846947946686</v>
+        <v>-0.08073292072730784</v>
       </c>
       <c r="AHB3">
-        <v>-0.08871675368052026</v>
+        <v>-0.08531405566488609</v>
       </c>
       <c r="AHC3">
-        <v>-0.09113979648925519</v>
+        <v>-0.0865786121777726</v>
       </c>
       <c r="AHD3">
-        <v>-0.09117036969272285</v>
+        <v>-0.08676489587056625</v>
       </c>
       <c r="AHE3">
-        <v>-0.0796369610749294</v>
+        <v>-0.08073108611445881</v>
       </c>
       <c r="AHF3">
-        <v>-0.08875310511863349</v>
+        <v>-0.08531512898308445</v>
       </c>
       <c r="AHG3">
-        <v>-0.08868750739447226</v>
+        <v>-0.08527444640410396</v>
       </c>
       <c r="AHH3">
-        <v>-0.09120278525089477</v>
+        <v>-0.0865888827068539</v>
       </c>
       <c r="AHI3">
-        <v>-0.07960998756487482</v>
+        <v>-0.08069827934595765</v>
       </c>
       <c r="AHJ3">
-        <v>-0.08881279264970846</v>
+        <v>-0.08531689128891891</v>
       </c>
       <c r="AHK3">
-        <v>-0.08866270220926871</v>
+        <v>-0.08524085198754203</v>
       </c>
       <c r="AHL3">
-        <v>-0.0914480188667125</v>
+        <v>-0.08662886620953093</v>
       </c>
       <c r="AHM3">
-        <v>-0.07944523666266483</v>
+        <v>-0.08053358564132657</v>
       </c>
       <c r="AHN3">
-        <v>-0.07963110411478008</v>
+        <v>-0.08070399814710226</v>
       </c>
       <c r="AHO3">
-        <v>-0.08882459439794262</v>
+        <v>-0.08531723973624583</v>
       </c>
       <c r="AHP3">
-        <v>-0.08862100895909085</v>
+        <v>-0.08518438577260744</v>
       </c>
       <c r="AHQ3">
-        <v>-0.09189358158649093</v>
+        <v>-0.08670150103364381</v>
       </c>
       <c r="AHR3">
-        <v>-0.07933582318272699</v>
+        <v>-0.08042421014714973</v>
       </c>
       <c r="AHS3">
-        <v>-0.08883456667597231</v>
+        <v>-0.08531753416693433</v>
       </c>
       <c r="AHT3">
-        <v>-0.08884297032055957</v>
+        <v>-0.08531778228284082</v>
       </c>
       <c r="AHU3">
-        <v>-0.08885390211433655</v>
+        <v>-0.08531810504046264</v>
       </c>
       <c r="AHV3">
-        <v>-0.08887368711220801</v>
+        <v>-0.08531868918205837</v>
       </c>
       <c r="AHW3">
-        <v>-0.08890799122494245</v>
+        <v>-0.08531970198071619</v>
       </c>
       <c r="AHX3">
-        <v>-0.08918900040955562</v>
+        <v>-0.0853279979499679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>